<commit_message>
2016-14-12 new comments from Thomas on the Failsave solution.
2016-14-12 new comments from Thomas on the Failsave solution.
</commit_message>
<xml_diff>
--- a/Gemalto-CloudGate-Issues_O.xlsx
+++ b/Gemalto-CloudGate-Issues_O.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="57">
   <si>
     <t>Issue</t>
   </si>
@@ -106,9 +106,6 @@
   <si>
     <t>•Is a CG Gemalto supposed to work fine with a CG 3G or LTE configuration file?
 •Requested a log file.</t>
-  </si>
-  <si>
-    <t>•Is a CG Gemalto supposed to work fine with a CG 3G or LTE configuration file?</t>
   </si>
   <si>
     <t>•Retest requested as per Resultion/Plan
@@ -197,6 +194,19 @@
   </si>
   <si>
     <t>Firewall rules not loading from a configuration file created on a CG 3G.</t>
+  </si>
+  <si>
+    <t>•Is a CG Gemalto supposed to work fine with a CG 3G or LTE configuration file?
+•It cannot be assumed that the CG 3G or CG LTE configuration files will work with the Gemalto CloudGate. This was the same between a CG 3G and a CG LTE.</t>
+  </si>
+  <si>
+    <t>○</t>
+  </si>
+  <si>
+    <t>•A configuration file made on a different CloudGate type will not work on any CloudGate. This was already the case with configuration files from a CG 3G placed on a CG LTE.</t>
+  </si>
+  <si>
+    <t>•The comment as before.  The firewall rules will certainly not be correct.</t>
   </si>
 </sst>
 </file>
@@ -317,7 +327,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="16">
     <dxf>
       <font>
         <b/>
@@ -358,6 +368,17 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -369,227 +390,18 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -995,8 +807,8 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,7 +839,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>9</v>
@@ -1056,16 +868,16 @@
         <v>3</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>23</v>
@@ -1085,16 +897,16 @@
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>23</v>
@@ -1114,16 +926,16 @@
         <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>23</v>
@@ -1143,13 +955,13 @@
         <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="7" t="s">
@@ -1170,13 +982,13 @@
         <v>7</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="7" t="s">
@@ -1197,13 +1009,13 @@
         <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="7" t="s">
@@ -1224,13 +1036,13 @@
         <v>10</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="7" t="s">
@@ -1251,13 +1063,13 @@
         <v>11</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="7" t="s">
@@ -1275,13 +1087,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -1295,20 +1107,22 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="F12" s="1"/>
       <c r="G12" s="7" t="s">
         <v>19</v>
@@ -1320,20 +1134,22 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="11">
-        <v>11</v>
+    <row r="13" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>54</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="F13" s="1"/>
       <c r="G13" s="7" t="s">
         <v>19</v>
@@ -1363,62 +1179,62 @@
   </sheetData>
   <autoFilter ref="G1:G14"/>
   <conditionalFormatting sqref="H3:H9">
-    <cfRule type="cellIs" dxfId="21" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="28" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="29" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="30" operator="equal">
       <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:H13">
-    <cfRule type="cellIs" dxfId="18" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="25" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="26" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="27" operator="equal">
       <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14">
-    <cfRule type="cellIs" dxfId="15" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="22" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="23" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="24" operator="equal">
       <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G14">
-    <cfRule type="expression" dxfId="12" priority="19">
+    <cfRule type="expression" dxfId="6" priority="19">
       <formula>ISNUMBER(SEARCH("Under",G3))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="20" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="21" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G14">
-    <cfRule type="cellIs" dxfId="9" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="18" operator="equal">
       <formula>"New firmware"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I14">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="8" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="9" operator="equal">
       <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Correct numbering of issue list
Correct numbering of issue list
</commit_message>
<xml_diff>
--- a/Gemalto-CloudGate-Issues_O.xlsx
+++ b/Gemalto-CloudGate-Issues_O.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="56">
   <si>
     <t>Issue</t>
   </si>
@@ -198,9 +198,6 @@
   <si>
     <t>•Is a CG Gemalto supposed to work fine with a CG 3G or LTE configuration file?
 •It cannot be assumed that the CG 3G or CG LTE configuration files will work with the Gemalto CloudGate. This was the same between a CG 3G and a CG LTE.</t>
-  </si>
-  <si>
-    <t>○</t>
   </si>
   <si>
     <t>•A configuration file made on a different CloudGate type will not work on any CloudGate. This was already the case with configuration files from a CG 3G placed on a CG LTE.</t>
@@ -808,7 +805,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1121,7 +1118,7 @@
         <v>28</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="7" t="s">
@@ -1135,8 +1132,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>54</v>
+      <c r="A13" s="11">
+        <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>52</v>
@@ -1148,7 +1145,7 @@
         <v>53</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="7" t="s">

</xml_diff>

<commit_message>
2016-12-14 Updates after call with GetWireless.
2016-12-14 Updates after call with GetWireless.
</commit_message>
<xml_diff>
--- a/Gemalto-CloudGate-Issues_O.xlsx
+++ b/Gemalto-CloudGate-Issues_O.xlsx
@@ -804,8 +804,8 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1095,7 +1095,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>16</v>
@@ -1122,7 +1122,7 @@
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>16</v>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Comments on items 10 and 11. Tested and working.
Comments on items 10 and 11. Tested and working.
</commit_message>
<xml_diff>
--- a/Gemalto-CloudGate-Issues_O.xlsx
+++ b/Gemalto-CloudGate-Issues_O.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="58">
   <si>
     <t>Issue</t>
   </si>
@@ -102,10 +102,6 @@
   </si>
   <si>
     <t>Reported by customer</t>
-  </si>
-  <si>
-    <t>•Is a CG Gemalto supposed to work fine with a CG 3G or LTE configuration file?
-•Requested a log file.</t>
   </si>
   <si>
     <t>•Retest requested as per Resultion/Plan
@@ -197,13 +193,28 @@
   </si>
   <si>
     <t>•Is a CG Gemalto supposed to work fine with a CG 3G or LTE configuration file?
-•It cannot be assumed that the CG 3G or CG LTE configuration files will work with the Gemalto CloudGate. This was the same between a CG 3G and a CG LTE.</t>
-  </si>
-  <si>
-    <t>•A configuration file made on a different CloudGate type will not work on any CloudGate. This was already the case with configuration files from a CG 3G placed on a CG LTE.</t>
-  </si>
-  <si>
-    <t>•The comment as before.  The firewall rules will certainly not be correct.</t>
+•Requested a log file.
+•Tested the configuration file and don't see the same on my device. I do see other items that might be related to the configuration file being done on a CG 3G.</t>
+  </si>
+  <si>
+    <t>•Is a CG Gemalto supposed to work fine with a CG 3G or LTE configuration file?
+•It cannot be assumed that the CG 3G or CG LTE configuration files will work with the Gemalto CloudGate. This was the same between a CG 3G and a CG LTE.
+•Tested the configuration file and don't see the same on my device. I do see other items that might be related to the configuration file being done on a CG 3G.</t>
+  </si>
+  <si>
+    <t>•A configuration file made on a different CloudGate type will not work on any CloudGate. This was already the case with configuration files from a CG 3G placed on a CG LTE.
+•12/14/ Not able to reproduce with my device and the configuratio file from the customer.</t>
+  </si>
+  <si>
+    <t>•The comment as before.  The firewall rules will certainly not be correct.
+•12/14/ Not able to reproduce with my device and the configuratio file from the customer.</t>
+  </si>
+  <si>
+    <t>•Asking for a log.
+•Giving suggestions to the customer.</t>
+  </si>
+  <si>
+    <t>•Giving suggestions to the customer.</t>
   </si>
 </sst>
 </file>
@@ -804,8 +815,8 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,7 +847,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>9</v>
@@ -865,16 +876,16 @@
         <v>3</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>23</v>
@@ -894,16 +905,16 @@
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>23</v>
@@ -923,16 +934,16 @@
         <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>23</v>
@@ -952,13 +963,13 @@
         <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="7" t="s">
@@ -979,13 +990,13 @@
         <v>7</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="7" t="s">
@@ -1006,13 +1017,13 @@
         <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="7" t="s">
@@ -1033,13 +1044,13 @@
         <v>10</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="7" t="s">
@@ -1060,13 +1071,13 @@
         <v>11</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="7" t="s">
@@ -1084,13 +1095,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -1104,25 +1115,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F12" s="1"/>
+      <c r="F12" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="G12" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>16</v>
@@ -1131,15 +1144,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>53</v>
@@ -1147,9 +1160,11 @@
       <c r="E13" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F13" s="1"/>
+      <c r="F13" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="G13" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
16/12/2016 Updates after talking with Thomas
16/12/2016 Updates after talking with Thomas
</commit_message>
<xml_diff>
--- a/Gemalto-CloudGate-Issues_O.xlsx
+++ b/Gemalto-CloudGate-Issues_O.xlsx
@@ -8,7 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="Issue Tracking" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Legend" sheetId="3" state="hidden" r:id="rId2"/>
+    <sheet name="Customer Feedback" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Issue Tracking'!$G$1:$G$14</definedName>
@@ -18,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="67">
   <si>
     <t>Issue</t>
   </si>
@@ -202,10 +203,6 @@
 •Tested the configuration file and don't see the same on my device. I do see other items that might be related to the configuration file being done on a CG 3G.</t>
   </si>
   <si>
-    <t>•A configuration file made on a different CloudGate type will not work on any CloudGate. This was already the case with configuration files from a CG 3G placed on a CG LTE.
-•12/14/ Not able to reproduce with my device and the configuratio file from the customer.</t>
-  </si>
-  <si>
     <t>•The comment as before.  The firewall rules will certainly not be correct.
 •12/14/ Not able to reproduce with my device and the configuratio file from the customer.</t>
   </si>
@@ -215,6 +212,39 @@
   </si>
   <si>
     <t>•Giving suggestions to the customer.</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Feedback</t>
+  </si>
+  <si>
+    <t>Stephen Neff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All goes well, the new CloudGate is working beautifully.  
+The only thing is the info that Kathy ask for.  We are having a meeting Friday and it would be fabulous if we had that regulatory info by then. </t>
+  </si>
+  <si>
+    <t>Chris Liebig</t>
+  </si>
+  <si>
+    <t>The screws are a more course thread with less threads which makes it quicker to remove and replace the plate covering the SIM slot. Also, when booted up it was either set for TMobile already or the device auto detected it. I have to login and make that setting change on the old ones  for it to take effect.  Connected fine and have controllers communicating just fine so far. CL to get more clarification.</t>
+  </si>
+  <si>
+    <t>Mike Hanzlik @ Modem Express</t>
+  </si>
+  <si>
+    <t>All testing has gone well for their data logger solutions, and they have no issues with the Gemalto 3g CloudGate.  It is being sent back to Modem Express.</t>
+  </si>
+  <si>
+    <t>•A configuration file made on a different CloudGate type will not work on any CloudGate. This was already the case with configuration files from a CG 3G placed on a CG LTE.
+•12/14/ Not able to reproduce with my device and the configuratio file from the customer.
+•12/15 Sent customer logs for verification with the App team.</t>
   </si>
 </sst>
 </file>
@@ -293,7 +323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -330,6 +360,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -816,7 +855,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,7 +1154,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>10</v>
       </c>
@@ -1129,13 +1168,13 @@
         <v>52</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>16</v>
@@ -1158,10 +1197,10 @@
         <v>53</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>20</v>
@@ -1257,19 +1296,19 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Sheet3!$B$2:$B$4</xm:f>
+            <xm:f>Legend!$B$2:$B$4</xm:f>
           </x14:formula1>
           <xm:sqref>H3:H14</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Sheet3!$C$2:$C$7</xm:f>
+            <xm:f>Legend!$C$2:$C$7</xm:f>
           </x14:formula1>
           <xm:sqref>G3:G14</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Sheet3!$D$2:$D$3</xm:f>
+            <xm:f>Legend!$D$2:$D$3</xm:f>
           </x14:formula1>
           <xm:sqref>I3:I14</xm:sqref>
         </x14:dataValidation>
@@ -1341,4 +1380,113 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="76.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="14">
+        <v>42710</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="14">
+        <v>42712</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="14">
+        <v>42717</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
19/12/2016 Update on the LuvitRED issue reported by Failsave.
19/12/2016 Update on the LuvitRED issue reported by Failsave.
</commit_message>
<xml_diff>
--- a/Gemalto-CloudGate-Issues_O.xlsx
+++ b/Gemalto-CloudGate-Issues_O.xlsx
@@ -194,11 +194,6 @@
   </si>
   <si>
     <t>•Is a CG Gemalto supposed to work fine with a CG 3G or LTE configuration file?
-•Requested a log file.
-•Tested the configuration file and don't see the same on my device. I do see other items that might be related to the configuration file being done on a CG 3G.</t>
-  </si>
-  <si>
-    <t>•Is a CG Gemalto supposed to work fine with a CG 3G or LTE configuration file?
 •It cannot be assumed that the CG 3G or CG LTE configuration files will work with the Gemalto CloudGate. This was the same between a CG 3G and a CG LTE.
 •Tested the configuration file and don't see the same on my device. I do see other items that might be related to the configuration file being done on a CG 3G.</t>
   </si>
@@ -242,9 +237,16 @@
     <t>All testing has gone well for their data logger solutions, and they have no issues with the Gemalto 3g CloudGate.  It is being sent back to Modem Express.</t>
   </si>
   <si>
+    <t>•Is a CG Gemalto supposed to work fine with a CG 3G or LTE configuration file?
+•Requested a log file.
+•Tested the configuration file and don't see the same on my device. I do see other items that might be related to the configuration file being done on a CG 3G.
+•Timothy suggested an update to LuvitRED 2.10.0 as there are some items included that might alliviate this, but the problem is certainly related to the configuration file being made on a different CG type.</t>
+  </si>
+  <si>
     <t>•A configuration file made on a different CloudGate type will not work on any CloudGate. This was already the case with configuration files from a CG 3G placed on a CG LTE.
 •12/14/ Not able to reproduce with my device and the configuratio file from the customer.
-•12/15 Sent customer logs for verification with the App team.</t>
+•12/15 Sent customer logs for verification with the App team.
+•12/19 Customer to try the latest LuvitRED 2.10.0, but more important to try a configuration file created on a CloudGate Gemalto.</t>
   </si>
 </sst>
 </file>
@@ -854,8 +856,8 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1154,7 +1156,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>10</v>
       </c>
@@ -1165,13 +1167,13 @@
         <v>49</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>66</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>22</v>
@@ -1194,13 +1196,13 @@
         <v>49</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="F13" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>20</v>
@@ -1399,46 +1401,46 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
         <v>57</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>58</v>
-      </c>
-      <c r="C2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="14">
         <v>42710</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4" s="14">
         <v>42712</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" s="14">
         <v>42717</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Change status of issue 10
Change status of issue 10
</commit_message>
<xml_diff>
--- a/Gemalto-CloudGate-Issues_O.xlsx
+++ b/Gemalto-CloudGate-Issues_O.xlsx
@@ -857,7 +857,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1176,7 +1176,7 @@
         <v>54</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
22/12/2016 Minor updates from call with Thomas.
22/12/2016 Minor updates from call with Thomas.
</commit_message>
<xml_diff>
--- a/Gemalto-CloudGate-Issues_O.xlsx
+++ b/Gemalto-CloudGate-Issues_O.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="68">
   <si>
     <t>Issue</t>
   </si>
@@ -198,10 +198,6 @@
 •Tested the configuration file and don't see the same on my device. I do see other items that might be related to the configuration file being done on a CG 3G.</t>
   </si>
   <si>
-    <t>•The comment as before.  The firewall rules will certainly not be correct.
-•12/14/ Not able to reproduce with my device and the configuratio file from the customer.</t>
-  </si>
-  <si>
     <t>•Asking for a log.
 •Giving suggestions to the customer.</t>
   </si>
@@ -243,10 +239,19 @@
 •Timothy suggested an update to LuvitRED 2.10.0 as there are some items included that might alliviate this, but the problem is certainly related to the configuration file being made on a different CG type.</t>
   </si>
   <si>
+    <t>•12/22 Brandon to Verify if this is the case.</t>
+  </si>
+  <si>
+    <t>•The comment as before.  The firewall rules will certainly not be correct.
+•12/14/ Not able to reproduce with my device and the configuratio file from the customer.
+•12/22 Can we close this item?</t>
+  </si>
+  <si>
     <t>•A configuration file made on a different CloudGate type will not work on any CloudGate. This was already the case with configuration files from a CG 3G placed on a CG LTE.
 •12/14/ Not able to reproduce with my device and the configuratio file from the customer.
 •12/15 Sent customer logs for verification with the App team.
-•12/19 Customer to try the latest LuvitRED 2.10.0, but more important to try a configuration file created on a CloudGate Gemalto.</t>
+•12/19 Customer to try the latest LuvitRED 2.10.0, but more important to try a configuration file created on a CloudGate Gemalto. 
+•12/22 Can we close this item?</t>
   </si>
 </sst>
 </file>
@@ -856,8 +861,8 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1144,7 +1149,9 @@
       <c r="D11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="F11" s="1"/>
       <c r="G11" s="7" t="s">
         <v>20</v>
@@ -1156,7 +1163,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="210" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>10</v>
       </c>
@@ -1167,13 +1174,13 @@
         <v>49</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>20</v>
@@ -1199,10 +1206,10 @@
         <v>52</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>20</v>
@@ -1401,46 +1408,46 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
         <v>56</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>57</v>
-      </c>
-      <c r="C2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" s="14">
         <v>42710</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="14">
         <v>42712</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" s="14">
         <v>42717</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
23/12/2016 Update from the Joint call with GetWireless.
23/12/2016 Update from the Joint call with GetWireless.
</commit_message>
<xml_diff>
--- a/Gemalto-CloudGate-Issues_O.xlsx
+++ b/Gemalto-CloudGate-Issues_O.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="85">
   <si>
     <t>Issue</t>
   </si>
@@ -137,27 +137,12 @@
     <t>•Action item assigned to Jimmy.</t>
   </si>
   <si>
-    <t>•Will be there in December probably the second week. We are still figuring out the date.</t>
-  </si>
-  <si>
-    <t>•According to Thomas the next release will include the CG0198 too. There is no date for that release yet as we want to include as many fixes as possible.
-•Release by second week of December (2.70.0).</t>
-  </si>
-  <si>
     <t>•Jimmy needs to have a teamviewer session to debug what is going on here.
 •28/11 Teamviewer ready for Jimmy.
 •29/11 Jimmy tested and saw a delay of 2 minutes when switching. He will investigate and see if there is any chance for improvement.
 •There is a problem with this setup being offline every day. Jimmy is loosing time as he cannot test without an active TV.</t>
   </si>
   <si>
-    <t>•This is the same on both the current CG 3G (Gobi) and the CG LTE. There was no change compared to those devices.
-•We will try to get to a solution for the release following the 2.70.0. Some testing will be needed from GetWireless and Option.
-•Engineering build will be provided in January for testing and if OK, then a release will happen the same month.</t>
-  </si>
-  <si>
-    <t>•Fix will be available on the next firmware release (2.70.0).</t>
-  </si>
-  <si>
     <t>•This is under investigation.
 •Sent some comments on the item back to GetWireless on Friday (25/11)</t>
   </si>
@@ -214,14 +199,8 @@
     <t>Feedback</t>
   </si>
   <si>
-    <t>Stephen Neff</t>
-  </si>
-  <si>
     <t xml:space="preserve">All goes well, the new CloudGate is working beautifully.  
 The only thing is the info that Kathy ask for.  We are having a meeting Friday and it would be fabulous if we had that regulatory info by then. </t>
-  </si>
-  <si>
-    <t>Chris Liebig</t>
   </si>
   <si>
     <t>The screws are a more course thread with less threads which makes it quicker to remove and replace the plate covering the SIM slot. Also, when booted up it was either set for TMobile already or the device auto detected it. I have to login and make that setting change on the old ones  for it to take effect.  Connected fine and have controllers communicating just fine so far. CL to get more clarification.</t>
@@ -252,6 +231,82 @@
 •12/15 Sent customer logs for verification with the App team.
 •12/19 Customer to try the latest LuvitRED 2.10.0, but more important to try a configuration file created on a CloudGate Gemalto. 
 •12/22 Can we close this item?</t>
+  </si>
+  <si>
+    <t>Stephen Neff @ Emerson PakSense</t>
+  </si>
+  <si>
+    <t>Chris Liebig @ Advantage Controls</t>
+  </si>
+  <si>
+    <t>Dave Defusco @ Sensaphone</t>
+  </si>
+  <si>
+    <t>“I’m not too impressed with the Gemalto-based modem. I’m seeing a lot of disconnects despite having a good signal (green LED). I’m also using a diversity antenna as well. I don’t recall seeing as many issues with other version.”</t>
+  </si>
+  <si>
+    <t>Testing Status</t>
+  </si>
+  <si>
+    <t>Happy and sending unit back;  Will next be sent to DigiFarms</t>
+  </si>
+  <si>
+    <t>Modem Express</t>
+  </si>
+  <si>
+    <t>Geosonics happy and returning the CloudGate to Modem Express;  Next going to Houston Electric for testing</t>
+  </si>
+  <si>
+    <t>Sensaphone</t>
+  </si>
+  <si>
+    <t>Not happy per comments above.  Brandon working with them to get a log of disconnects</t>
+  </si>
+  <si>
+    <t>Failsafe</t>
+  </si>
+  <si>
+    <t>Waiting for them to create a new template and retest</t>
+  </si>
+  <si>
+    <t>BiPOM</t>
+  </si>
+  <si>
+    <t>Had some connection persistence questions and Franco responded.  Waiting on results.</t>
+  </si>
+  <si>
+    <t>Valmont</t>
+  </si>
+  <si>
+    <t>Could not test because did not have a Verizon plan.  GetWireless added our 3G Verizon plan earlier this week, but no update yet.</t>
+  </si>
+  <si>
+    <t>Emerson-PakSense</t>
+  </si>
+  <si>
+    <t>Happy per comments above and Steve Koontz working to get it returned</t>
+  </si>
+  <si>
+    <t>Tom Hoyt testing over the Holidays</t>
+  </si>
+  <si>
+    <t>•Fix will be available on the next firmware release (2.70.0).
+•12/23 Due to lack of people during the Christmas period the release will only happening the first week of January.</t>
+  </si>
+  <si>
+    <t>•This is the same on both the current CG 3G (Gobi) and the CG LTE. There was no change compared to those devices.
+•We will try to get to a solution for the release following the 2.70.0. Some testing will be needed from GetWireless and Option.
+•Engineering build will be provided in January for testing and if OK, then a release will happen the same month.
+•12/23 Due to lack of people during the Christmas period the release will only happening the first week of January.</t>
+  </si>
+  <si>
+    <t>•According to Thomas the next release will include the CG0198 too. There is no date for that release yet as we want to include as many fixes as possible.
+•Release by second week of December (2.70.0).
+•12/23 Due to lack of people during the Christmas period the release will only happening the first week of January.</t>
+  </si>
+  <si>
+    <t>•Will be there in December probably the second week. We are still figuring out the date.
+•12/23 Due to lack of people during the Christmas period the release will only happening the first week of January.</t>
   </si>
 </sst>
 </file>
@@ -330,7 +385,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -374,9 +429,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -861,8 +917,8 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,7 +949,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>9</v>
@@ -922,16 +978,16 @@
         <v>3</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>23</v>
@@ -951,16 +1007,16 @@
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>29</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>23</v>
@@ -980,16 +1036,16 @@
         <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>29</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>23</v>
@@ -1001,7 +1057,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>4</v>
       </c>
@@ -1009,13 +1065,13 @@
         <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="7" t="s">
@@ -1036,13 +1092,13 @@
         <v>7</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="7" t="s">
@@ -1063,13 +1119,13 @@
         <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="7" t="s">
@@ -1082,7 +1138,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>7</v>
       </c>
@@ -1090,13 +1146,13 @@
         <v>10</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="7" t="s">
@@ -1109,7 +1165,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>8</v>
       </c>
@@ -1117,13 +1173,13 @@
         <v>11</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>36</v>
+        <v>84</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="7" t="s">
@@ -1141,16 +1197,16 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="7" t="s">
@@ -1168,19 +1224,19 @@
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>20</v>
@@ -1197,19 +1253,19 @@
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>20</v>
@@ -1393,107 +1449,155 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C14"/>
+  <dimension ref="A2:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="76.28515625" customWidth="1"/>
+    <col min="3" max="3" width="117.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B3" s="14">
         <v>42710</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B4" s="14">
         <v>42712</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B5" s="14">
         <v>42717</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="14">
+        <v>42726</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-    </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
+      <c r="A9" s="15" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
+      <c r="A11" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
+      <c r="A12" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
+      <c r="A13" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
+      <c r="A14" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16" t="s">
+        <v>80</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
04/01/2017 Update after call with Thomas
04/01/2017 Update after call with Thomas
</commit_message>
<xml_diff>
--- a/Gemalto-CloudGate-Issues_O.xlsx
+++ b/Gemalto-CloudGate-Issues_O.xlsx
@@ -294,12 +294,6 @@
 •12/23 Due to lack of people during the Christmas period the release will only happening the first week of January.</t>
   </si>
   <si>
-    <t>•This is the same on both the current CG 3G (Gobi) and the CG LTE. There was no change compared to those devices.
-•We will try to get to a solution for the release following the 2.70.0. Some testing will be needed from GetWireless and Option.
-•Engineering build will be provided in January for testing and if OK, then a release will happen the same month.
-•12/23 Due to lack of people during the Christmas period the release will only happening the first week of January.</t>
-  </si>
-  <si>
     <t>•According to Thomas the next release will include the CG0198 too. There is no date for that release yet as we want to include as many fixes as possible.
 •Release by second week of December (2.70.0).
 •12/23 Due to lack of people during the Christmas period the release will only happening the first week of January.</t>
@@ -307,6 +301,11 @@
   <si>
     <t>•Will be there in December probably the second week. We are still figuring out the date.
 •12/23 Due to lack of people during the Christmas period the release will only happening the first week of January.</t>
+  </si>
+  <si>
+    <t>•This is the same on both the current CG 3G (Gobi) and the CG LTE. There was no change compared to those devices.
+•We will try to get to a solution for the release following the 2.70.0. Some testing will be needed from GetWireless and Option.
+•Engineering build will be provided in January for testing and if OK, then a release will happen the same month.</t>
   </si>
 </sst>
 </file>
@@ -914,11 +913,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,7 +970,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>1</v>
       </c>
@@ -999,7 +999,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>2</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>3</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>31</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="7" t="s">
@@ -1152,7 +1152,7 @@
         <v>33</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="7" t="s">
@@ -1179,7 +1179,7 @@
         <v>34</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="7" t="s">
@@ -1293,7 +1293,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="G1:G14"/>
+  <autoFilter ref="G1:G14">
+    <filterColumn colId="0">
+      <filters blank="1">
+        <filter val="New firmware"/>
+        <filter val="Status"/>
+        <filter val="Under Test (GW)"/>
+        <filter val="Under Test (OP)"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="H3:H9">
     <cfRule type="cellIs" dxfId="15" priority="28" operator="equal">
       <formula>"Low"</formula>
@@ -1452,7 +1461,7 @@
   <dimension ref="A2:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
04/01/2017 Update after GW call.
04/01/2017 Update after GW call.
</commit_message>
<xml_diff>
--- a/Gemalto-CloudGate-Issues_O.xlsx
+++ b/Gemalto-CloudGate-Issues_O.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="86">
   <si>
     <t>Issue</t>
   </si>
@@ -137,12 +137,6 @@
     <t>•Action item assigned to Jimmy.</t>
   </si>
   <si>
-    <t>•Jimmy needs to have a teamviewer session to debug what is going on here.
-•28/11 Teamviewer ready for Jimmy.
-•29/11 Jimmy tested and saw a delay of 2 minutes when switching. He will investigate and see if there is any chance for improvement.
-•There is a problem with this setup being offline every day. Jimmy is loosing time as he cannot test without an active TV.</t>
-  </si>
-  <si>
     <t>•This is under investigation.
 •Sent some comments on the item back to GetWireless on Friday (25/11)</t>
   </si>
@@ -216,9 +210,6 @@
 •Requested a log file.
 •Tested the configuration file and don't see the same on my device. I do see other items that might be related to the configuration file being done on a CG 3G.
 •Timothy suggested an update to LuvitRED 2.10.0 as there are some items included that might alliviate this, but the problem is certainly related to the configuration file being made on a different CG type.</t>
-  </si>
-  <si>
-    <t>•12/22 Brandon to Verify if this is the case.</t>
   </si>
   <si>
     <t>•The comment as before.  The firewall rules will certainly not be correct.
@@ -306,6 +297,20 @@
     <t>•This is the same on both the current CG 3G (Gobi) and the CG LTE. There was no change compared to those devices.
 •We will try to get to a solution for the release following the 2.70.0. Some testing will be needed from GetWireless and Option.
 •Engineering build will be provided in January for testing and if OK, then a release will happen the same month.</t>
+  </si>
+  <si>
+    <t>Under Test (Customer)</t>
+  </si>
+  <si>
+    <t>•Jimmy needs to have a teamviewer session to debug what is going on here.
+•11/28 Teamviewer ready for Jimmy.
+•11/29 Jimmy tested and saw a delay of 2 minutes when switching. He will investigate and see if there is any chance for improvement.
+•There is a problem with this setup being offline every day. Jimmy is loosing time as he cannot test without an active TV.
+•01/04 Jimmy is going to try to see the same issue in Belgium and if he does the TV setup will no longer be needed.</t>
+  </si>
+  <si>
+    <t>•12/22 Brandon to Verify if this is the case.
+•01/04 Brandon is waiting for his device to come back in order to test this.</t>
   </si>
 </sst>
 </file>
@@ -917,8 +922,8 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -949,7 +954,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>9</v>
@@ -978,16 +983,16 @@
         <v>3</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>23</v>
@@ -1007,16 +1012,16 @@
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>29</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>23</v>
@@ -1036,16 +1041,16 @@
         <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>29</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>23</v>
@@ -1065,13 +1070,13 @@
         <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="7" t="s">
@@ -1092,13 +1097,13 @@
         <v>7</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="7" t="s">
@@ -1111,7 +1116,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>6</v>
       </c>
@@ -1119,13 +1124,13 @@
         <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>36</v>
+        <v>84</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="7" t="s">
@@ -1146,13 +1151,13 @@
         <v>10</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="7" t="s">
@@ -1173,13 +1178,13 @@
         <v>11</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="7" t="s">
@@ -1197,16 +1202,16 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="7" t="s">
@@ -1224,22 +1229,22 @@
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>20</v>
+        <v>83</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>16</v>
@@ -1253,22 +1258,22 @@
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="E13" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>20</v>
+        <v>83</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>16</v>
@@ -1376,7 +1381,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Legend!$C$2:$C$7</xm:f>
+            <xm:f>Legend!$C$2:$C$8</xm:f>
           </x14:formula1>
           <xm:sqref>G3:G14</xm:sqref>
         </x14:dataValidation>
@@ -1394,10 +1399,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D7"/>
+  <dimension ref="B2:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1448,6 +1453,11 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1473,57 +1483,57 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
         <v>51</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>52</v>
-      </c>
-      <c r="C2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B3" s="14">
         <v>42710</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B4" s="14">
         <v>42712</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" s="14">
         <v>42717</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B6" s="14">
         <v>42726</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1533,79 +1543,79 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" s="16"/>
       <c r="C11" s="16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B12" s="16"/>
       <c r="C12" s="16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B13" s="16"/>
       <c r="C13" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B14" s="16"/>
       <c r="C14" s="16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B15" s="16"/>
       <c r="C15" s="16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B16" s="16"/>
       <c r="C16" s="16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B17" s="16"/>
       <c r="C17" s="16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" s="16"/>
       <c r="C18" s="16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
06/01/2017 Updates after local testing.
06/01/2017 Updates after local testing.
</commit_message>
<xml_diff>
--- a/Gemalto-CloudGate-Issues_O.xlsx
+++ b/Gemalto-CloudGate-Issues_O.xlsx
@@ -212,11 +212,6 @@
 •Timothy suggested an update to LuvitRED 2.10.0 as there are some items included that might alliviate this, but the problem is certainly related to the configuration file being made on a different CG type.</t>
   </si>
   <si>
-    <t>•The comment as before.  The firewall rules will certainly not be correct.
-•12/14/ Not able to reproduce with my device and the configuratio file from the customer.
-•12/22 Can we close this item?</t>
-  </si>
-  <si>
     <t>•A configuration file made on a different CloudGate type will not work on any CloudGate. This was already the case with configuration files from a CG 3G placed on a CG LTE.
 •12/14/ Not able to reproduce with my device and the configuratio file from the customer.
 •12/15 Sent customer logs for verification with the App team.
@@ -281,10 +276,6 @@
     <t>Tom Hoyt testing over the Holidays</t>
   </si>
   <si>
-    <t>•Fix will be available on the next firmware release (2.70.0).
-•12/23 Due to lack of people during the Christmas period the release will only happening the first week of January.</t>
-  </si>
-  <si>
     <t>•According to Thomas the next release will include the CG0198 too. There is no date for that release yet as we want to include as many fixes as possible.
 •Release by second week of December (2.70.0).
 •12/23 Due to lack of people during the Christmas period the release will only happening the first week of January.</t>
@@ -292,11 +283,6 @@
   <si>
     <t>•Will be there in December probably the second week. We are still figuring out the date.
 •12/23 Due to lack of people during the Christmas period the release will only happening the first week of January.</t>
-  </si>
-  <si>
-    <t>•This is the same on both the current CG 3G (Gobi) and the CG LTE. There was no change compared to those devices.
-•We will try to get to a solution for the release following the 2.70.0. Some testing will be needed from GetWireless and Option.
-•Engineering build will be provided in January for testing and if OK, then a release will happen the same month.</t>
   </si>
   <si>
     <t>Under Test (Customer)</t>
@@ -311,6 +297,23 @@
   <si>
     <t>•12/22 Brandon to Verify if this is the case.
 •01/04 Brandon is waiting for his device to come back in order to test this.</t>
+  </si>
+  <si>
+    <t>•The comment as before.  The firewall rules will certainly not be correct.
+•12/14/ Not able to reproduce with my device and the configuratio file from the customer.
+•12/22 Can we close this item?
+•01/06 Tested the last report from the customer regarding the port forwarding rule not working together with the rule of LuvitRED and I have not found the issue the customer is reporting.</t>
+  </si>
+  <si>
+    <t>•Fix will be available on the next firmware release (2.70.0).
+•12/23 Due to lack of people during the Christmas period the release will only happening the first week of January.
+•01/06 Seems to be fixed on the 2.70.0 firmware. GetWireless to confirm.</t>
+  </si>
+  <si>
+    <t>•This is the same on both the current CG 3G (Gobi) and the CG LTE. There was no change compared to those devices.
+•We will try to get to a solution for the release following the 2.70.0. Some testing will be needed from GetWireless and Option.
+•Engineering build will be provided in January for testing and if OK, then a release will happen the same month.
+•01/06 Engineering build provided to GetWireless. GetWireless to test.</t>
   </si>
 </sst>
 </file>
@@ -922,8 +925,8 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,7 +1065,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>4</v>
       </c>
@@ -1076,7 +1079,7 @@
         <v>30</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="7" t="s">
@@ -1103,11 +1106,11 @@
         <v>31</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>17</v>
@@ -1130,7 +1133,7 @@
         <v>32</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="7" t="s">
@@ -1157,11 +1160,11 @@
         <v>33</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>15</v>
@@ -1184,7 +1187,7 @@
         <v>34</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="7" t="s">
@@ -1211,7 +1214,7 @@
         <v>35</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="7" t="s">
@@ -1224,7 +1227,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>10</v>
       </c>
@@ -1238,13 +1241,13 @@
         <v>57</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>48</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>83</v>
+        <v>23</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>16</v>
@@ -1267,13 +1270,13 @@
         <v>47</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>49</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>83</v>
+        <v>20</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>16</v>
@@ -1453,7 +1456,7 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
@@ -1494,7 +1497,7 @@
     </row>
     <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="14">
         <v>42710</v>
@@ -1505,7 +1508,7 @@
     </row>
     <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="14">
         <v>42712</v>
@@ -1527,13 +1530,13 @@
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" s="14">
         <v>42726</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1543,7 +1546,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1552,61 +1555,61 @@
       </c>
       <c r="B11" s="16"/>
       <c r="C11" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B12" s="16"/>
       <c r="C12" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B13" s="16"/>
       <c r="C13" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B14" s="16"/>
       <c r="C14" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B15" s="16"/>
       <c r="C15" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B16" s="16"/>
       <c r="C16" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B17" s="16"/>
       <c r="C17" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1615,7 +1618,7 @@
       </c>
       <c r="B18" s="16"/>
       <c r="C18" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
11/01/2017 Updates from Friday and after call with Thomas.
11/01/2017 Updates from Friday and after call with Thomas.
</commit_message>
<xml_diff>
--- a/Gemalto-CloudGate-Issues_O.xlsx
+++ b/Gemalto-CloudGate-Issues_O.xlsx
@@ -122,11 +122,6 @@
 Call with Thomas and Jimmy, we will try to include a solution on the next release of firmware (not 2.70.0, but the one after that one)</t>
   </si>
   <si>
-    <t>•Jimmy requested a Teamviewer session. Franco to work on getting this setup.
-•28/11 TV ready for Jimmy.
-•29/11 Jimmy tested today and saw a delay of 2 minutes to find a signal. He will investigate.</t>
-  </si>
-  <si>
     <t>•2.70.0 is going to be the first Gemalto firmware.</t>
   </si>
   <si>
@@ -288,32 +283,40 @@
     <t>Under Test (Customer)</t>
   </si>
   <si>
+    <t>•12/22 Brandon to Verify if this is the case.
+•01/04 Brandon is waiting for his device to come back in order to test this.</t>
+  </si>
+  <si>
+    <t>•The comment as before.  The firewall rules will certainly not be correct.
+•12/14/ Not able to reproduce with my device and the configuratio file from the customer.
+•12/22 Can we close this item?
+•01/06 Tested the last report from the customer regarding the port forwarding rule not working together with the rule of LuvitRED and I have not found the issue the customer is reporting.</t>
+  </si>
+  <si>
+    <t>•Fix will be available on the next firmware release (2.70.0).
+•12/23 Due to lack of people during the Christmas period the release will only happening the first week of January.
+•01/06 Seems to be fixed on the 2.70.0 firmware. GetWireless to confirm.</t>
+  </si>
+  <si>
+    <t>•Jimmy requested a Teamviewer session. Franco to work on getting this setup.
+•28/11 TV ready for Jimmy.
+•29/11 Jimmy tested today and saw a delay of 2 minutes to find a signal. He will investigate.
+•11/01 Does not seem to be related to the firmware switch. but to a specific SIM. We are asking Gemalto to check this on the modem.</t>
+  </si>
+  <si>
+    <t>•This is the same on both the current CG 3G (Gobi) and the CG LTE. There was no change compared to those devices.
+•We will try to get to a solution for the release following the 2.70.0. Some testing will be needed from GetWireless and Option.
+•Engineering build will be provided in January for testing and if OK, then a release will happen the same month.
+•01/06 Engineering build provided to GetWireless. GetWireless to test.
+•01/11 It will be great if we can get a result by the end of the week so that we can add it on the release candidate.</t>
+  </si>
+  <si>
     <t>•Jimmy needs to have a teamviewer session to debug what is going on here.
 •11/28 Teamviewer ready for Jimmy.
 •11/29 Jimmy tested and saw a delay of 2 minutes when switching. He will investigate and see if there is any chance for improvement.
 •There is a problem with this setup being offline every day. Jimmy is loosing time as he cannot test without an active TV.
-•01/04 Jimmy is going to try to see the same issue in Belgium and if he does the TV setup will no longer be needed.</t>
-  </si>
-  <si>
-    <t>•12/22 Brandon to Verify if this is the case.
-•01/04 Brandon is waiting for his device to come back in order to test this.</t>
-  </si>
-  <si>
-    <t>•The comment as before.  The firewall rules will certainly not be correct.
-•12/14/ Not able to reproduce with my device and the configuratio file from the customer.
-•12/22 Can we close this item?
-•01/06 Tested the last report from the customer regarding the port forwarding rule not working together with the rule of LuvitRED and I have not found the issue the customer is reporting.</t>
-  </si>
-  <si>
-    <t>•Fix will be available on the next firmware release (2.70.0).
-•12/23 Due to lack of people during the Christmas period the release will only happening the first week of January.
-•01/06 Seems to be fixed on the 2.70.0 firmware. GetWireless to confirm.</t>
-  </si>
-  <si>
-    <t>•This is the same on both the current CG 3G (Gobi) and the CG LTE. There was no change compared to those devices.
-•We will try to get to a solution for the release following the 2.70.0. Some testing will be needed from GetWireless and Option.
-•Engineering build will be provided in January for testing and if OK, then a release will happen the same month.
-•01/06 Engineering build provided to GetWireless. GetWireless to test.</t>
+•01/04 Jimmy is going to try to see the same issue in Belgium and if he does the TV setup will no longer be needed.
+•01/11 The issue does not seem to be related to the firmware switch, but to something specific on the SIM. We are asking Gemalto to check this on the module.</t>
   </si>
 </sst>
 </file>
@@ -925,8 +928,8 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,7 +960,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>9</v>
@@ -986,16 +989,16 @@
         <v>3</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>23</v>
@@ -1015,16 +1018,16 @@
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>29</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>23</v>
@@ -1044,16 +1047,16 @@
         <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>29</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>23</v>
@@ -1073,13 +1076,13 @@
         <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="7" t="s">
@@ -1100,13 +1103,13 @@
         <v>7</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="7" t="s">
@@ -1119,7 +1122,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="255" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>6</v>
       </c>
@@ -1127,13 +1130,13 @@
         <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="7" t="s">
@@ -1154,13 +1157,13 @@
         <v>10</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="7" t="s">
@@ -1181,17 +1184,17 @@
         <v>11</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>15</v>
@@ -1205,16 +1208,16 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="7" t="s">
@@ -1232,19 +1235,19 @@
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="F12" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>23</v>
@@ -1261,19 +1264,19 @@
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="E13" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>20</v>
@@ -1456,7 +1459,7 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
@@ -1486,57 +1489,57 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
         <v>50</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>51</v>
-      </c>
-      <c r="C2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" s="14">
         <v>42710</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" s="14">
         <v>42712</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" s="14">
         <v>42717</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6" s="14">
         <v>42726</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1546,79 +1549,79 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" s="16"/>
       <c r="C11" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B12" s="16"/>
       <c r="C12" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B13" s="16"/>
       <c r="C13" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B14" s="16"/>
       <c r="C14" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B15" s="16"/>
       <c r="C15" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B16" s="16"/>
       <c r="C16" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B17" s="16"/>
       <c r="C17" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" s="16"/>
       <c r="C18" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
13/01/2017 Update after GetWireless call.
13/01/2017 Update after GetWireless call.
</commit_message>
<xml_diff>
--- a/Gemalto-CloudGate-Issues_O.xlsx
+++ b/Gemalto-CloudGate-Issues_O.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="75">
   <si>
     <t>Issue</t>
   </si>
@@ -179,9 +179,6 @@
     <t>•Giving suggestions to the customer.</t>
   </si>
   <si>
-    <t>Contact</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -193,9 +190,6 @@
   </si>
   <si>
     <t>The screws are a more course thread with less threads which makes it quicker to remove and replace the plate covering the SIM slot. Also, when booted up it was either set for TMobile already or the device auto detected it. I have to login and make that setting change on the old ones  for it to take effect.  Connected fine and have controllers communicating just fine so far. CL to get more clarification.</t>
-  </si>
-  <si>
-    <t>Mike Hanzlik @ Modem Express</t>
   </si>
   <si>
     <t>All testing has gone well for their data logger solutions, and they have no issues with the Gemalto 3g CloudGate.  It is being sent back to Modem Express.</t>
@@ -214,61 +208,13 @@
 •12/22 Can we close this item?</t>
   </si>
   <si>
-    <t>Stephen Neff @ Emerson PakSense</t>
-  </si>
-  <si>
-    <t>Chris Liebig @ Advantage Controls</t>
-  </si>
-  <si>
-    <t>Dave Defusco @ Sensaphone</t>
-  </si>
-  <si>
     <t>“I’m not too impressed with the Gemalto-based modem. I’m seeing a lot of disconnects despite having a good signal (green LED). I’m also using a diversity antenna as well. I don’t recall seeing as many issues with other version.”</t>
   </si>
   <si>
-    <t>Testing Status</t>
-  </si>
-  <si>
     <t>Happy and sending unit back;  Will next be sent to DigiFarms</t>
   </si>
   <si>
-    <t>Modem Express</t>
-  </si>
-  <si>
-    <t>Geosonics happy and returning the CloudGate to Modem Express;  Next going to Houston Electric for testing</t>
-  </si>
-  <si>
-    <t>Sensaphone</t>
-  </si>
-  <si>
-    <t>Not happy per comments above.  Brandon working with them to get a log of disconnects</t>
-  </si>
-  <si>
-    <t>Failsafe</t>
-  </si>
-  <si>
-    <t>Waiting for them to create a new template and retest</t>
-  </si>
-  <si>
-    <t>BiPOM</t>
-  </si>
-  <si>
     <t>Had some connection persistence questions and Franco responded.  Waiting on results.</t>
-  </si>
-  <si>
-    <t>Valmont</t>
-  </si>
-  <si>
-    <t>Could not test because did not have a Verizon plan.  GetWireless added our 3G Verizon plan earlier this week, but no update yet.</t>
-  </si>
-  <si>
-    <t>Emerson-PakSense</t>
-  </si>
-  <si>
-    <t>Happy per comments above and Steve Koontz working to get it returned</t>
-  </si>
-  <si>
-    <t>Tom Hoyt testing over the Holidays</t>
   </si>
   <si>
     <t>•According to Thomas the next release will include the CG0198 too. There is no date for that release yet as we want to include as many fixes as possible.
@@ -318,12 +264,33 @@
 •01/04 Jimmy is going to try to see the same issue in Belgium and if he does the TV setup will no longer be needed.
 •01/11 The issue does not seem to be related to the firmware switch, but to something specific on the SIM. We are asking Gemalto to check this on the module.</t>
   </si>
+  <si>
+    <t>After getting Verizon connectivity, testing has gone well.  Just confirming they are finished with their unit.  Returned their unit.  Shipped to Wanco.</t>
+  </si>
+  <si>
+    <t>Happy per comments above and device is returned.  Shipped to Pinnacle.</t>
+  </si>
+  <si>
+    <t>Per Jim Wagner on Tuesday 1/10/2017:  Mike and I spoke and UPS lost the package from Geosonics so Houston Electric has not seen the device yet. UPS found the package and delivered it today to Modem Express. The package was beat up, but the CloudGate looks good. They are sending it to Houston Electric tomorrow via 2 Day so they should have it on Friday.</t>
+  </si>
+  <si>
+    <t>No response from Sensaphone on request to send back unit.  Truax following up.</t>
+  </si>
+  <si>
+    <t>Customer uses port forwarding to open up port 4000 on CG firewall; however when the TCP node in LuvitRED already opens the hole in the firewall on that port, serial device is not reachable.  He is retesting with Gobi based CloudGate per Franco's input.</t>
+  </si>
+  <si>
+    <t>No update as of yet.</t>
+  </si>
+  <si>
+    <t>Brandon testing</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -346,16 +313,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -391,11 +369,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -439,10 +428,20 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -928,8 +927,8 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <pane ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1082,11 +1081,11 @@
         <v>30</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>16</v>
@@ -1109,7 +1108,7 @@
         <v>31</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="7" t="s">
@@ -1133,10 +1132,10 @@
         <v>40</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="7" t="s">
@@ -1149,7 +1148,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>7</v>
       </c>
@@ -1163,7 +1162,7 @@
         <v>32</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="7" t="s">
@@ -1176,7 +1175,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>8</v>
       </c>
@@ -1190,7 +1189,7 @@
         <v>33</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="7" t="s">
@@ -1217,7 +1216,7 @@
         <v>34</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="7" t="s">
@@ -1241,10 +1240,10 @@
         <v>43</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>47</v>
@@ -1273,7 +1272,7 @@
         <v>46</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>48</v>
@@ -1459,7 +1458,7 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
@@ -1474,19 +1473,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C18"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="117.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="134.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="117.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1"/>
+      <c r="B1"/>
+    </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>49</v>
@@ -1494,134 +1498,128 @@
       <c r="B2" t="s">
         <v>50</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
+        <v>42710</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="B3" s="14">
-        <v>42710</v>
-      </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="22"/>
+    </row>
+    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="14">
+        <v>42712</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" s="14">
-        <v>42712</v>
-      </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="22"/>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="14">
+        <v>42717</v>
+      </c>
+      <c r="B5" s="13" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="14">
-        <v>42717</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>55</v>
-      </c>
+      <c r="C5" s="22"/>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" s="14">
+      <c r="A6" s="14">
         <v>42726</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>61</v>
-      </c>
+      <c r="B6" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="22"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
+      <c r="C7" s="22"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8"/>
+      <c r="B8"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>62</v>
-      </c>
+      <c r="A9"/>
+      <c r="B9"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10"/>
+      <c r="B10"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16" t="s">
-        <v>63</v>
-      </c>
+      <c r="A11"/>
+      <c r="B11"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16" t="s">
-        <v>65</v>
+      <c r="A12" s="16"/>
+      <c r="B12" s="16" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16" t="s">
-        <v>67</v>
+      <c r="A13" s="16"/>
+      <c r="B13" s="16" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16" t="s">
+      <c r="A14" s="16"/>
+      <c r="B14" s="16" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
+    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
+      <c r="B15" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16" t="s">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
+      <c r="B16" s="15" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="B17" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16" t="s">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
+      <c r="B18" s="15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="19"/>
+      <c r="B19" s="20" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
+      <c r="B20" s="20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="15"/>
+      <c r="B21" s="20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="15"/>
+      <c r="B22" s="15" t="s">
         <v>74</v>
-      </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
18/01/2017 Updates from call with Thomas and Jimmy.
18/01/2017 Updates from call with Thomas and Jimmy.
</commit_message>
<xml_diff>
--- a/Gemalto-CloudGate-Issues_O.xlsx
+++ b/Gemalto-CloudGate-Issues_O.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="76">
   <si>
     <t>Issue</t>
   </si>
@@ -244,17 +244,25 @@
 •01/06 Seems to be fixed on the 2.70.0 firmware. GetWireless to confirm.</t>
   </si>
   <si>
-    <t>•Jimmy requested a Teamviewer session. Franco to work on getting this setup.
-•28/11 TV ready for Jimmy.
-•29/11 Jimmy tested today and saw a delay of 2 minutes to find a signal. He will investigate.
-•11/01 Does not seem to be related to the firmware switch. but to a specific SIM. We are asking Gemalto to check this on the modem.</t>
-  </si>
-  <si>
-    <t>•This is the same on both the current CG 3G (Gobi) and the CG LTE. There was no change compared to those devices.
-•We will try to get to a solution for the release following the 2.70.0. Some testing will be needed from GetWireless and Option.
-•Engineering build will be provided in January for testing and if OK, then a release will happen the same month.
-•01/06 Engineering build provided to GetWireless. GetWireless to test.
-•01/11 It will be great if we can get a result by the end of the week so that we can add it on the release candidate.</t>
+    <t>After getting Verizon connectivity, testing has gone well.  Just confirming they are finished with their unit.  Returned their unit.  Shipped to Wanco.</t>
+  </si>
+  <si>
+    <t>Happy per comments above and device is returned.  Shipped to Pinnacle.</t>
+  </si>
+  <si>
+    <t>Per Jim Wagner on Tuesday 1/10/2017:  Mike and I spoke and UPS lost the package from Geosonics so Houston Electric has not seen the device yet. UPS found the package and delivered it today to Modem Express. The package was beat up, but the CloudGate looks good. They are sending it to Houston Electric tomorrow via 2 Day so they should have it on Friday.</t>
+  </si>
+  <si>
+    <t>No response from Sensaphone on request to send back unit.  Truax following up.</t>
+  </si>
+  <si>
+    <t>Customer uses port forwarding to open up port 4000 on CG firewall; however when the TCP node in LuvitRED already opens the hole in the firewall on that port, serial device is not reachable.  He is retesting with Gobi based CloudGate per Franco's input.</t>
+  </si>
+  <si>
+    <t>No update as of yet.</t>
+  </si>
+  <si>
+    <t>Brandon testing</t>
   </si>
   <si>
     <t>•Jimmy needs to have a teamviewer session to debug what is going on here.
@@ -262,28 +270,26 @@
 •11/29 Jimmy tested and saw a delay of 2 minutes when switching. He will investigate and see if there is any chance for improvement.
 •There is a problem with this setup being offline every day. Jimmy is loosing time as he cannot test without an active TV.
 •01/04 Jimmy is going to try to see the same issue in Belgium and if he does the TV setup will no longer be needed.
-•01/11 The issue does not seem to be related to the firmware switch, but to something specific on the SIM. We are asking Gemalto to check this on the module.</t>
-  </si>
-  <si>
-    <t>After getting Verizon connectivity, testing has gone well.  Just confirming they are finished with their unit.  Returned their unit.  Shipped to Wanco.</t>
-  </si>
-  <si>
-    <t>Happy per comments above and device is returned.  Shipped to Pinnacle.</t>
-  </si>
-  <si>
-    <t>Per Jim Wagner on Tuesday 1/10/2017:  Mike and I spoke and UPS lost the package from Geosonics so Houston Electric has not seen the device yet. UPS found the package and delivered it today to Modem Express. The package was beat up, but the CloudGate looks good. They are sending it to Houston Electric tomorrow via 2 Day so they should have it on Friday.</t>
-  </si>
-  <si>
-    <t>No response from Sensaphone on request to send back unit.  Truax following up.</t>
-  </si>
-  <si>
-    <t>Customer uses port forwarding to open up port 4000 on CG firewall; however when the TCP node in LuvitRED already opens the hole in the firewall on that port, serial device is not reachable.  He is retesting with Gobi based CloudGate per Franco's input.</t>
-  </si>
-  <si>
-    <t>No update as of yet.</t>
-  </si>
-  <si>
-    <t>Brandon testing</t>
+•01/11 The issue does not seem to be related to the firmware switch, but to something specific on the SIM. We are asking Gemalto to check this on the module.
+•01/18 We are waiting feedback from Gemalto on this one. They are looking into it, but might take time.</t>
+  </si>
+  <si>
+    <t>•01/13 Brandon saw a problem with the modem not reading the SIM correctly after switching it and rebooting the modem.</t>
+  </si>
+  <si>
+    <t>•This is the same on both the current CG 3G (Gobi) and the CG LTE. There was no change compared to those devices.
+•We will try to get to a solution for the release following the 2.70.0. Some testing will be needed from GetWireless and Option.
+•Engineering build will be provided in January for testing and if OK, then a release will happen the same month.
+•01/06 Engineering build provided to GetWireless. GetWireless to test.
+•01/11 It will be great if we can get a result by the end of the week so that we can add it on the release candidate.
+•01/18 Jimmy is looking into this one.</t>
+  </si>
+  <si>
+    <t>•Jimmy requested a Teamviewer session. Franco to work on getting this setup.
+•28/11 TV ready for Jimmy.
+•29/11 Jimmy tested today and saw a delay of 2 minutes to find a signal. He will investigate.
+•11/01 Does not seem to be related to the firmware switch. but to a specific SIM. We are asking Gemalto to check this on the modem.
+•01/18 We are waiting feedback from Gemalto on this one. They are looking into it, but might take time.</t>
   </si>
 </sst>
 </file>
@@ -927,8 +933,8 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <pane ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1108,11 +1114,13 @@
         <v>31</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F7" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="G7" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>17</v>
@@ -1121,7 +1129,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="255" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="300" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>6</v>
       </c>
@@ -1132,10 +1140,10 @@
         <v>40</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="7" t="s">
@@ -1565,31 +1573,31 @@
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
       <c r="B13" s="16" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="16"/>
       <c r="B14" s="16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15" s="17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
       <c r="B16" s="15" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" s="18" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1601,25 +1609,25 @@
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="19"/>
       <c r="B19" s="20" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
       <c r="B20" s="20" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
       <c r="B21" s="20" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="15"/>
       <c r="B22" s="15" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20/01/2017 Minor updates on document.
20/01/2017 Minor updates on document.
</commit_message>
<xml_diff>
--- a/Gemalto-CloudGate-Issues_O.xlsx
+++ b/Gemalto-CloudGate-Issues_O.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="91">
   <si>
     <t>Issue</t>
   </si>
@@ -290,6 +290,51 @@
 •29/11 Jimmy tested today and saw a delay of 2 minutes to find a signal. He will investigate.
 •11/01 Does not seem to be related to the firmware switch. but to a specific SIM. We are asking Gemalto to check this on the modem.
 •01/18 We are waiting feedback from Gemalto on this one. They are looking into it, but might take time.</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Stephen Neff @ Emerson PakSense</t>
+  </si>
+  <si>
+    <t>Chris Liebig @ Advantage Controls</t>
+  </si>
+  <si>
+    <t>Mike Hanzlik @ Modem Express</t>
+  </si>
+  <si>
+    <t>Dave Defusco @ Sensaphone</t>
+  </si>
+  <si>
+    <t>Testing Status</t>
+  </si>
+  <si>
+    <t>Valmont</t>
+  </si>
+  <si>
+    <t>Emerson-PakSense</t>
+  </si>
+  <si>
+    <t>Modem Express</t>
+  </si>
+  <si>
+    <t>Sensaphone</t>
+  </si>
+  <si>
+    <t>Failsafe (JW)</t>
+  </si>
+  <si>
+    <t>BiPOM</t>
+  </si>
+  <si>
+    <t>DigiFarms</t>
+  </si>
+  <si>
+    <t>Pinnacle IP</t>
+  </si>
+  <si>
+    <t>Wanco</t>
   </si>
 </sst>
 </file>
@@ -390,7 +435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -428,6 +473,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -444,8 +491,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -634,9 +680,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -933,8 +976,8 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1147,7 +1190,7 @@
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>16</v>
@@ -1484,149 +1527,199 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="134.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="117.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="21"/>
+    <col min="1" max="2" width="10.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="134.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1"/>
-      <c r="B1"/>
+      <c r="A1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="14" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="14">
+    <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="16">
         <v>42710</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="C3" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="22"/>
-    </row>
-    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="14">
+    </row>
+    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="16">
         <v>42712</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="C4" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="22"/>
-    </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="14">
+    </row>
+    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="16">
         <v>42717</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="C5" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="22"/>
-    </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="14">
+    </row>
+    <row r="6" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="16">
         <v>42726</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="C6" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="22"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="22"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8"/>
-      <c r="B8"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9"/>
-      <c r="B9"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10"/>
-      <c r="B10"/>
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11"/>
-      <c r="B11"/>
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16" t="s">
+      <c r="A12" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16" t="s">
+      <c r="A13" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16" t="s">
+      <c r="A14" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="17" t="s">
+      <c r="A15" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="17"/>
+      <c r="C15" s="19" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15" t="s">
+      <c r="A16" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="18" t="s">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" s="17"/>
+      <c r="C17" s="20" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
-      <c r="B19" s="20" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="21"/>
+      <c r="C19" s="22" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-      <c r="B20" s="20" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" s="17"/>
+      <c r="C20" s="22" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
-      <c r="B21" s="20" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" s="17"/>
+      <c r="C21" s="22" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>

<commit_message>
25/01/2017 Update after GW call
25/01/2017 Update after GW call
</commit_message>
<xml_diff>
--- a/Gemalto-CloudGate-Issues_O.xlsx
+++ b/Gemalto-CloudGate-Issues_O.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="92">
   <si>
     <t>Issue</t>
   </si>
@@ -170,13 +170,6 @@
     <t>•Is a CG Gemalto supposed to work fine with a CG 3G or LTE configuration file?
 •It cannot be assumed that the CG 3G or CG LTE configuration files will work with the Gemalto CloudGate. This was the same between a CG 3G and a CG LTE.
 •Tested the configuration file and don't see the same on my device. I do see other items that might be related to the configuration file being done on a CG 3G.</t>
-  </si>
-  <si>
-    <t>•Asking for a log.
-•Giving suggestions to the customer.</t>
-  </si>
-  <si>
-    <t>•Giving suggestions to the customer.</t>
   </si>
   <si>
     <t>Date</t>
@@ -277,64 +270,74 @@
     <t>•01/13 Brandon saw a problem with the modem not reading the SIM correctly after switching it and rebooting the modem.</t>
   </si>
   <si>
+    <t>•Jimmy requested a Teamviewer session. Franco to work on getting this setup.
+•28/11 TV ready for Jimmy.
+•29/11 Jimmy tested today and saw a delay of 2 minutes to find a signal. He will investigate.
+•11/01 Does not seem to be related to the firmware switch. but to a specific SIM. We are asking Gemalto to check this on the modem.
+•01/18 We are waiting feedback from Gemalto on this one. They are looking into it, but might take time.</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Stephen Neff @ Emerson PakSense</t>
+  </si>
+  <si>
+    <t>Chris Liebig @ Advantage Controls</t>
+  </si>
+  <si>
+    <t>Mike Hanzlik @ Modem Express</t>
+  </si>
+  <si>
+    <t>Dave Defusco @ Sensaphone</t>
+  </si>
+  <si>
+    <t>Testing Status</t>
+  </si>
+  <si>
+    <t>Valmont</t>
+  </si>
+  <si>
+    <t>Emerson-PakSense</t>
+  </si>
+  <si>
+    <t>Modem Express</t>
+  </si>
+  <si>
+    <t>Sensaphone</t>
+  </si>
+  <si>
+    <t>Failsafe (JW)</t>
+  </si>
+  <si>
+    <t>BiPOM</t>
+  </si>
+  <si>
+    <t>DigiFarms</t>
+  </si>
+  <si>
+    <t>Pinnacle IP</t>
+  </si>
+  <si>
+    <t>Wanco</t>
+  </si>
+  <si>
+    <t>•01/24 Brandon sees no issue in testing with 2.71.</t>
+  </si>
+  <si>
+    <t>•01/24 The modem does not auto detect the SIM and load the UMTS firmware. The modem default must be UMTS causing this behavior. The gobi default was Verizon.</t>
+  </si>
+  <si>
+    <t>•01/24 Brandon saw no problem with the firewall and LuvitRED opening the same port.</t>
+  </si>
+  <si>
     <t>•This is the same on both the current CG 3G (Gobi) and the CG LTE. There was no change compared to those devices.
 •We will try to get to a solution for the release following the 2.70.0. Some testing will be needed from GetWireless and Option.
 •Engineering build will be provided in January for testing and if OK, then a release will happen the same month.
 •01/06 Engineering build provided to GetWireless. GetWireless to test.
 •01/11 It will be great if we can get a result by the end of the week so that we can add it on the release candidate.
-•01/18 Jimmy is looking into this one.</t>
-  </si>
-  <si>
-    <t>•Jimmy requested a Teamviewer session. Franco to work on getting this setup.
-•28/11 TV ready for Jimmy.
-•29/11 Jimmy tested today and saw a delay of 2 minutes to find a signal. He will investigate.
-•11/01 Does not seem to be related to the firmware switch. but to a specific SIM. We are asking Gemalto to check this on the modem.
-•01/18 We are waiting feedback from Gemalto on this one. They are looking into it, but might take time.</t>
-  </si>
-  <si>
-    <t>Contact</t>
-  </si>
-  <si>
-    <t>Stephen Neff @ Emerson PakSense</t>
-  </si>
-  <si>
-    <t>Chris Liebig @ Advantage Controls</t>
-  </si>
-  <si>
-    <t>Mike Hanzlik @ Modem Express</t>
-  </si>
-  <si>
-    <t>Dave Defusco @ Sensaphone</t>
-  </si>
-  <si>
-    <t>Testing Status</t>
-  </si>
-  <si>
-    <t>Valmont</t>
-  </si>
-  <si>
-    <t>Emerson-PakSense</t>
-  </si>
-  <si>
-    <t>Modem Express</t>
-  </si>
-  <si>
-    <t>Sensaphone</t>
-  </si>
-  <si>
-    <t>Failsafe (JW)</t>
-  </si>
-  <si>
-    <t>BiPOM</t>
-  </si>
-  <si>
-    <t>DigiFarms</t>
-  </si>
-  <si>
-    <t>Pinnacle IP</t>
-  </si>
-  <si>
-    <t>Wanco</t>
+•01/18 Jimmy is looking into this one.
+•01/25 There seems to be a problem with the modem that stays on SIM not ready and that is why is showing the problem after a radio modem reboot. We need to look ino the modem log and either fix it ourselves or get a fix from Gemalto.</t>
   </si>
 </sst>
 </file>
@@ -435,7 +438,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -493,6 +496,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -975,9 +984,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1116,7 +1125,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>4</v>
       </c>
@@ -1130,11 +1139,13 @@
         <v>30</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F6" s="1"/>
+        <v>62</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>88</v>
+      </c>
       <c r="G6" s="7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>16</v>
@@ -1143,7 +1154,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="240" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="315" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>5</v>
       </c>
@@ -1157,10 +1168,10 @@
         <v>31</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>22</v>
@@ -1183,10 +1194,10 @@
         <v>40</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="7" t="s">
@@ -1213,7 +1224,7 @@
         <v>32</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="7" t="s">
@@ -1240,7 +1251,7 @@
         <v>33</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="7" t="s">
@@ -1253,7 +1264,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>9</v>
       </c>
@@ -1267,11 +1278,13 @@
         <v>34</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F11" s="1"/>
+        <v>60</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>89</v>
+      </c>
       <c r="G11" s="7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>16</v>
@@ -1291,13 +1304,13 @@
         <v>43</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>90</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>23</v>
@@ -1323,10 +1336,10 @@
         <v>46</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>48</v>
+        <v>90</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>20</v>
@@ -1357,10 +1370,9 @@
   <autoFilter ref="G1:G14">
     <filterColumn colId="0">
       <filters blank="1">
-        <filter val="New firmware"/>
         <filter val="Status"/>
+        <filter val="Under Investigation (OP)"/>
         <filter val="Under Test (GW)"/>
-        <filter val="Under Test (OP)"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -1509,7 +1521,7 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
@@ -1544,57 +1556,57 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B3" s="16">
         <v>42710</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B4" s="16">
         <v>42712</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B5" s="16">
         <v>42717</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B6" s="16">
         <v>42726</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1614,7 +1626,7 @@
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
@@ -1630,88 +1642,88 @@
       </c>
       <c r="B12" s="18"/>
       <c r="C12" s="18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B13" s="18"/>
       <c r="C13" s="18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B14" s="18"/>
       <c r="C14" s="18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B15" s="17"/>
       <c r="C15" s="19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B16" s="17"/>
       <c r="C16" s="17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B18" s="17"/>
       <c r="C18" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B19" s="21"/>
       <c r="C19" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B20" s="17"/>
       <c r="C20" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1720,7 +1732,7 @@
       </c>
       <c r="B22" s="17"/>
       <c r="C22" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
27/01/2017 Update after the GetWireless team call.
27/01/2017 Update after the GetWireless team call.
</commit_message>
<xml_diff>
--- a/Gemalto-CloudGate-Issues_O.xlsx
+++ b/Gemalto-CloudGate-Issues_O.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="94">
   <si>
     <t>Issue</t>
   </si>
@@ -207,9 +207,6 @@
     <t>Happy and sending unit back;  Will next be sent to DigiFarms</t>
   </si>
   <si>
-    <t>Had some connection persistence questions and Franco responded.  Waiting on results.</t>
-  </si>
-  <si>
     <t>•According to Thomas the next release will include the CG0198 too. There is no date for that release yet as we want to include as many fixes as possible.
 •Release by second week of December (2.70.0).
 •12/23 Due to lack of people during the Christmas period the release will only happening the first week of January.</t>
@@ -241,15 +238,6 @@
   </si>
   <si>
     <t>Happy per comments above and device is returned.  Shipped to Pinnacle.</t>
-  </si>
-  <si>
-    <t>Per Jim Wagner on Tuesday 1/10/2017:  Mike and I spoke and UPS lost the package from Geosonics so Houston Electric has not seen the device yet. UPS found the package and delivered it today to Modem Express. The package was beat up, but the CloudGate looks good. They are sending it to Houston Electric tomorrow via 2 Day so they should have it on Friday.</t>
-  </si>
-  <si>
-    <t>No response from Sensaphone on request to send back unit.  Truax following up.</t>
-  </si>
-  <si>
-    <t>Customer uses port forwarding to open up port 4000 on CG firewall; however when the TCP node in LuvitRED already opens the hole in the firewall on that port, serial device is not reachable.  He is retesting with Gobi based CloudGate per Franco's input.</t>
   </si>
   <si>
     <t>No update as of yet.</t>
@@ -338,6 +326,24 @@
 •01/11 It will be great if we can get a result by the end of the week so that we can add it on the release candidate.
 •01/18 Jimmy is looking into this one.
 •01/25 There seems to be a problem with the modem that stays on SIM not ready and that is why is showing the problem after a radio modem reboot. We need to look ino the modem log and either fix it ourselves or get a fix from Gemalto.</t>
+  </si>
+  <si>
+    <t>Houston Electric reported no issues.  En route back to GetWireless.</t>
+  </si>
+  <si>
+    <t>Still no response from Sensaphone on request to send back unit.  Brandon pinging them daily and Truax following up.</t>
+  </si>
+  <si>
+    <t>Customer uses port forwarding to open up port 4000 on CG firewall; however when the TCP node in LuvitRED already opens the hole in the firewall on that port, serial device is not reachable.  He is retesting with Gobi based CloudGate per Franco's input. Offshore most of last week- just getting back to more testing.</t>
+  </si>
+  <si>
+    <t>Being used for a project design. Jonathan working to free it up and get it back.</t>
+  </si>
+  <si>
+    <t>Passed their tests.  Andrew working on tracking down if sent back yet.</t>
+  </si>
+  <si>
+    <t>Having challenges activating on Verizon after GetWireless removed their Verizon plan.  Factory reseting not helping.  Brandon engaged.</t>
   </si>
 </sst>
 </file>
@@ -387,7 +393,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -434,11 +440,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -485,13 +517,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -503,6 +528,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1139,10 +1176,10 @@
         <v>30</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F6" s="24" t="s">
-        <v>88</v>
+        <v>61</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>84</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>23</v>
@@ -1168,10 +1205,10 @@
         <v>31</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>22</v>
@@ -1194,10 +1231,10 @@
         <v>40</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="7" t="s">
@@ -1224,7 +1261,7 @@
         <v>32</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="7" t="s">
@@ -1251,7 +1288,7 @@
         <v>33</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="7" t="s">
@@ -1278,10 +1315,10 @@
         <v>34</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F11" s="25" t="s">
-        <v>89</v>
+        <v>59</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>85</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>23</v>
@@ -1309,8 +1346,8 @@
       <c r="E12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="25" t="s">
-        <v>90</v>
+      <c r="F12" s="22" t="s">
+        <v>86</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>23</v>
@@ -1336,10 +1373,10 @@
         <v>46</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>20</v>
@@ -1521,7 +1558,7 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
@@ -1539,13 +1576,14 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="134.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="133.28515625" style="13" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
@@ -1555,19 +1593,19 @@
       <c r="C1" s="14"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" s="14" t="s">
+      <c r="A2" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="23" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B3" s="16">
         <v>42710</v>
@@ -1578,7 +1616,7 @@
     </row>
     <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B4" s="16">
         <v>42712</v>
@@ -1589,7 +1627,7 @@
     </row>
     <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B5" s="16">
         <v>42717</v>
@@ -1598,9 +1636,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B6" s="16">
         <v>42726</v>
@@ -1625,8 +1663,8 @@
       <c r="C9" s="14"/>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
-        <v>78</v>
+      <c r="A10" s="20" t="s">
+        <v>74</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
@@ -1637,93 +1675,93 @@
       <c r="C11" s="14"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18" t="s">
+      <c r="B12" s="25"/>
+      <c r="C12" s="29" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18" t="s">
+      <c r="A13" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="30"/>
+      <c r="C13" s="25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B15" s="17"/>
-      <c r="C15" s="19" t="s">
-        <v>65</v>
+      <c r="C15" s="26" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B16" s="17"/>
-      <c r="C16" s="17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="C16" s="24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B17" s="17"/>
-      <c r="C17" s="20" t="s">
-        <v>67</v>
+      <c r="C17" s="27" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B18" s="17"/>
-      <c r="C18" s="17" t="s">
-        <v>56</v>
+      <c r="C18" s="24" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="22" t="s">
-        <v>68</v>
+      <c r="A19" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="18"/>
+      <c r="C19" s="28" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
-        <v>86</v>
+      <c r="A20" s="19" t="s">
+        <v>82</v>
       </c>
       <c r="B20" s="17"/>
-      <c r="C20" s="22" t="s">
-        <v>68</v>
+      <c r="C20" s="28" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
-        <v>87</v>
+      <c r="A21" s="19" t="s">
+        <v>83</v>
       </c>
       <c r="B21" s="17"/>
-      <c r="C21" s="22" t="s">
-        <v>68</v>
+      <c r="C21" s="28" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1731,11 +1769,12 @@
         <v>40</v>
       </c>
       <c r="B22" s="17"/>
-      <c r="C22" s="17" t="s">
-        <v>69</v>
+      <c r="C22" s="24" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
01/02/2017 Update from the BE team on items 5 and 6.
01/02/2017 Update from the BE team on items 5 and 6.
</commit_message>
<xml_diff>
--- a/Gemalto-CloudGate-Issues_O.xlsx
+++ b/Gemalto-CloudGate-Issues_O.xlsx
@@ -246,77 +246,96 @@
     <t>Brandon testing</t>
   </si>
   <si>
+    <t>•01/13 Brandon saw a problem with the modem not reading the SIM correctly after switching it and rebooting the modem.</t>
+  </si>
+  <si>
+    <t>•Jimmy requested a Teamviewer session. Franco to work on getting this setup.
+•28/11 TV ready for Jimmy.
+•29/11 Jimmy tested today and saw a delay of 2 minutes to find a signal. He will investigate.
+•11/01 Does not seem to be related to the firmware switch. but to a specific SIM. We are asking Gemalto to check this on the modem.
+•01/18 We are waiting feedback from Gemalto on this one. They are looking into it, but might take time.</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Stephen Neff @ Emerson PakSense</t>
+  </si>
+  <si>
+    <t>Chris Liebig @ Advantage Controls</t>
+  </si>
+  <si>
+    <t>Mike Hanzlik @ Modem Express</t>
+  </si>
+  <si>
+    <t>Dave Defusco @ Sensaphone</t>
+  </si>
+  <si>
+    <t>Testing Status</t>
+  </si>
+  <si>
+    <t>Valmont</t>
+  </si>
+  <si>
+    <t>Emerson-PakSense</t>
+  </si>
+  <si>
+    <t>Modem Express</t>
+  </si>
+  <si>
+    <t>Sensaphone</t>
+  </si>
+  <si>
+    <t>Failsafe (JW)</t>
+  </si>
+  <si>
+    <t>BiPOM</t>
+  </si>
+  <si>
+    <t>DigiFarms</t>
+  </si>
+  <si>
+    <t>Pinnacle IP</t>
+  </si>
+  <si>
+    <t>Wanco</t>
+  </si>
+  <si>
+    <t>•01/24 Brandon sees no issue in testing with 2.71.</t>
+  </si>
+  <si>
+    <t>•01/24 The modem does not auto detect the SIM and load the UMTS firmware. The modem default must be UMTS causing this behavior. The gobi default was Verizon.</t>
+  </si>
+  <si>
+    <t>•01/24 Brandon saw no problem with the firewall and LuvitRED opening the same port.</t>
+  </si>
+  <si>
+    <t>Houston Electric reported no issues.  En route back to GetWireless.</t>
+  </si>
+  <si>
+    <t>Still no response from Sensaphone on request to send back unit.  Brandon pinging them daily and Truax following up.</t>
+  </si>
+  <si>
+    <t>Customer uses port forwarding to open up port 4000 on CG firewall; however when the TCP node in LuvitRED already opens the hole in the firewall on that port, serial device is not reachable.  He is retesting with Gobi based CloudGate per Franco's input. Offshore most of last week- just getting back to more testing.</t>
+  </si>
+  <si>
+    <t>Being used for a project design. Jonathan working to free it up and get it back.</t>
+  </si>
+  <si>
+    <t>Passed their tests.  Andrew working on tracking down if sent back yet.</t>
+  </si>
+  <si>
+    <t>Having challenges activating on Verizon after GetWireless removed their Verizon plan.  Factory reseting not helping.  Brandon engaged.</t>
+  </si>
+  <si>
     <t>•Jimmy needs to have a teamviewer session to debug what is going on here.
 •11/28 Teamviewer ready for Jimmy.
 •11/29 Jimmy tested and saw a delay of 2 minutes when switching. He will investigate and see if there is any chance for improvement.
 •There is a problem with this setup being offline every day. Jimmy is loosing time as he cannot test without an active TV.
 •01/04 Jimmy is going to try to see the same issue in Belgium and if he does the TV setup will no longer be needed.
 •01/11 The issue does not seem to be related to the firmware switch, but to something specific on the SIM. We are asking Gemalto to check this on the module.
-•01/18 We are waiting feedback from Gemalto on this one. They are looking into it, but might take time.</t>
-  </si>
-  <si>
-    <t>•01/13 Brandon saw a problem with the modem not reading the SIM correctly after switching it and rebooting the modem.</t>
-  </si>
-  <si>
-    <t>•Jimmy requested a Teamviewer session. Franco to work on getting this setup.
-•28/11 TV ready for Jimmy.
-•29/11 Jimmy tested today and saw a delay of 2 minutes to find a signal. He will investigate.
-•11/01 Does not seem to be related to the firmware switch. but to a specific SIM. We are asking Gemalto to check this on the modem.
-•01/18 We are waiting feedback from Gemalto on this one. They are looking into it, but might take time.</t>
-  </si>
-  <si>
-    <t>Contact</t>
-  </si>
-  <si>
-    <t>Stephen Neff @ Emerson PakSense</t>
-  </si>
-  <si>
-    <t>Chris Liebig @ Advantage Controls</t>
-  </si>
-  <si>
-    <t>Mike Hanzlik @ Modem Express</t>
-  </si>
-  <si>
-    <t>Dave Defusco @ Sensaphone</t>
-  </si>
-  <si>
-    <t>Testing Status</t>
-  </si>
-  <si>
-    <t>Valmont</t>
-  </si>
-  <si>
-    <t>Emerson-PakSense</t>
-  </si>
-  <si>
-    <t>Modem Express</t>
-  </si>
-  <si>
-    <t>Sensaphone</t>
-  </si>
-  <si>
-    <t>Failsafe (JW)</t>
-  </si>
-  <si>
-    <t>BiPOM</t>
-  </si>
-  <si>
-    <t>DigiFarms</t>
-  </si>
-  <si>
-    <t>Pinnacle IP</t>
-  </si>
-  <si>
-    <t>Wanco</t>
-  </si>
-  <si>
-    <t>•01/24 Brandon sees no issue in testing with 2.71.</t>
-  </si>
-  <si>
-    <t>•01/24 The modem does not auto detect the SIM and load the UMTS firmware. The modem default must be UMTS causing this behavior. The gobi default was Verizon.</t>
-  </si>
-  <si>
-    <t>•01/24 Brandon saw no problem with the firewall and LuvitRED opening the same port.</t>
+•01/18 We are waiting feedback from Gemalto on this one. They are looking into it, but might take time.
+•02/01 Gemalto is asking for a new, more complicated log to get some more data about the issue, but this log is proving to be a complicated one. The BE team is working to get the log for them.</t>
   </si>
   <si>
     <t>•This is the same on both the current CG 3G (Gobi) and the CG LTE. There was no change compared to those devices.
@@ -325,25 +344,8 @@
 •01/06 Engineering build provided to GetWireless. GetWireless to test.
 •01/11 It will be great if we can get a result by the end of the week so that we can add it on the release candidate.
 •01/18 Jimmy is looking into this one.
-•01/25 There seems to be a problem with the modem that stays on SIM not ready and that is why is showing the problem after a radio modem reboot. We need to look ino the modem log and either fix it ourselves or get a fix from Gemalto.</t>
-  </si>
-  <si>
-    <t>Houston Electric reported no issues.  En route back to GetWireless.</t>
-  </si>
-  <si>
-    <t>Still no response from Sensaphone on request to send back unit.  Brandon pinging them daily and Truax following up.</t>
-  </si>
-  <si>
-    <t>Customer uses port forwarding to open up port 4000 on CG firewall; however when the TCP node in LuvitRED already opens the hole in the firewall on that port, serial device is not reachable.  He is retesting with Gobi based CloudGate per Franco's input. Offshore most of last week- just getting back to more testing.</t>
-  </si>
-  <si>
-    <t>Being used for a project design. Jonathan working to free it up and get it back.</t>
-  </si>
-  <si>
-    <t>Passed their tests.  Andrew working on tracking down if sent back yet.</t>
-  </si>
-  <si>
-    <t>Having challenges activating on Verizon after GetWireless removed their Verizon plan.  Factory reseting not helping.  Brandon engaged.</t>
+•01/25 There seems to be a problem with the modem that stays on SIM not ready and that is why is showing the problem after a radio modem reboot. We need to look ino the modem log and either fix it ourselves or get a fix from Gemalto.
+• 02/01 The BE team is still investigating the reason why the SIM command returns "SIM busy" after the modem reboot. It is not clear yet why this is happening. More investigation is needed.</t>
   </si>
 </sst>
 </file>
@@ -1023,7 +1025,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,7 +1041,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="27" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="5"/>
@@ -1179,7 +1181,7 @@
         <v>61</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>23</v>
@@ -1191,7 +1193,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="315" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="390" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>5</v>
       </c>
@@ -1205,22 +1207,22 @@
         <v>31</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>22</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="300" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="375" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>6</v>
       </c>
@@ -1231,10 +1233,10 @@
         <v>40</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="7" t="s">
@@ -1318,7 +1320,7 @@
         <v>59</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>23</v>
@@ -1347,7 +1349,7 @@
         <v>53</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>23</v>
@@ -1359,7 +1361,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <v>11</v>
       </c>
@@ -1376,10 +1378,10 @@
         <v>60</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>16</v>
@@ -1409,7 +1411,6 @@
       <filters blank="1">
         <filter val="Status"/>
         <filter val="Under Investigation (OP)"/>
-        <filter val="Under Test (GW)"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -1576,7 +1577,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1594,7 +1595,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" s="23" t="s">
         <v>47</v>
@@ -1605,7 +1606,7 @@
     </row>
     <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="16">
         <v>42710</v>
@@ -1616,7 +1617,7 @@
     </row>
     <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" s="16">
         <v>42712</v>
@@ -1627,7 +1628,7 @@
     </row>
     <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5" s="16">
         <v>42717</v>
@@ -1638,7 +1639,7 @@
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B6" s="16">
         <v>42726</v>
@@ -1664,7 +1665,7 @@
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
@@ -1685,7 +1686,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B13" s="30"/>
       <c r="C13" s="25" t="s">
@@ -1694,7 +1695,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B14" s="25"/>
       <c r="C14" s="25" t="s">
@@ -1703,52 +1704,52 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B15" s="17"/>
       <c r="C15" s="26" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B16" s="17"/>
       <c r="C16" s="24" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="27" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B18" s="17"/>
       <c r="C18" s="24" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B19" s="18"/>
       <c r="C19" s="28" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B20" s="17"/>
       <c r="C20" s="28" t="s">
@@ -1757,11 +1758,11 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="28" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
03/02/2017 Update after GetWireless call.
03/02/2017 Update after GetWireless call.
</commit_message>
<xml_diff>
--- a/Gemalto-CloudGate-Issues_O.xlsx
+++ b/Gemalto-CloudGate-Issues_O.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="96">
   <si>
     <t>Issue</t>
   </si>
@@ -326,16 +326,6 @@
   </si>
   <si>
     <t>Having challenges activating on Verizon after GetWireless removed their Verizon plan.  Factory reseting not helping.  Brandon engaged.</t>
-  </si>
-  <si>
-    <t>•Jimmy needs to have a teamviewer session to debug what is going on here.
-•11/28 Teamviewer ready for Jimmy.
-•11/29 Jimmy tested and saw a delay of 2 minutes when switching. He will investigate and see if there is any chance for improvement.
-•There is a problem with this setup being offline every day. Jimmy is loosing time as he cannot test without an active TV.
-•01/04 Jimmy is going to try to see the same issue in Belgium and if he does the TV setup will no longer be needed.
-•01/11 The issue does not seem to be related to the firmware switch, but to something specific on the SIM. We are asking Gemalto to check this on the module.
-•01/18 We are waiting feedback from Gemalto on this one. They are looking into it, but might take time.
-•02/01 Gemalto is asking for a new, more complicated log to get some more data about the issue, but this log is proving to be a complicated one. The BE team is working to get the log for them.</t>
   </si>
   <si>
     <t>•This is the same on both the current CG 3G (Gobi) and the CG LTE. There was no change compared to those devices.
@@ -346,6 +336,23 @@
 •01/18 Jimmy is looking into this one.
 •01/25 There seems to be a problem with the modem that stays on SIM not ready and that is why is showing the problem after a radio modem reboot. We need to look ino the modem log and either fix it ourselves or get a fix from Gemalto.
 • 02/01 The BE team is still investigating the reason why the SIM command returns "SIM busy" after the modem reboot. It is not clear yet why this is happening. More investigation is needed.</t>
+  </si>
+  <si>
+    <t>•Jimmy needs to have a teamviewer session to debug what is going on here.
+•11/28 Teamviewer ready for Jimmy.
+•11/29 Jimmy tested and saw a delay of 2 minutes when switching. He will investigate and see if there is any chance for improvement.
+•There is a problem with this setup being offline every day. Jimmy is loosing time as he cannot test without an active TV.
+•01/04 Jimmy is going to try to see the same issue in Belgium and if he does the TV setup will no longer be needed.
+•01/11 The issue does not seem to be related to the firmware switch, but to something specific on the SIM. We are asking Gemalto to check this on the module.
+•01/18 We are waiting feedback from Gemalto on this one. They are looking into it, but might take time.
+•02/01 Gemalto is asking for a new, more complicated log to get some more data about the issue, but this log is proving to be a complicated one. The BE team is working to get the log for them.
+•02/03 We sent a new log as requested by Gemalto.</t>
+  </si>
+  <si>
+    <t>New unit sent to them to evaluate; problem unit received back and being evaluated</t>
+  </si>
+  <si>
+    <t>Available.</t>
   </si>
 </sst>
 </file>
@@ -472,7 +479,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -511,6 +518,18 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -524,22 +543,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -1023,9 +1031,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1041,7 +1049,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="16" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="5"/>
@@ -1180,7 +1188,7 @@
       <c r="E6" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="14" t="s">
         <v>83</v>
       </c>
       <c r="G6" s="7" t="s">
@@ -1207,7 +1215,7 @@
         <v>31</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>66</v>
@@ -1222,7 +1230,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="375" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="405" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>6</v>
       </c>
@@ -1236,7 +1244,7 @@
         <v>67</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="7" t="s">
@@ -1319,7 +1327,7 @@
       <c r="E11" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="F11" s="15" t="s">
         <v>84</v>
       </c>
       <c r="G11" s="7" t="s">
@@ -1348,7 +1356,7 @@
       <c r="E12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="F12" s="15" t="s">
         <v>85</v>
       </c>
       <c r="G12" s="7" t="s">
@@ -1574,7 +1582,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
@@ -1589,190 +1597,206 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="14"/>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
+      <c r="A1" s="18"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="25" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="20">
         <v>42710</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="19" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="20">
         <v>42712</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="19" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="20">
         <v>42717</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="19" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="20">
         <v>42726</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="19" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-    </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A9" s="18"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="29" t="s">
+      <c r="B12" s="26"/>
+      <c r="C12" s="28" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="30"/>
-      <c r="C13" s="25" t="s">
+      <c r="B13" s="29"/>
+      <c r="C13" s="26" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25" t="s">
+      <c r="B14" s="26"/>
+      <c r="C14" s="26" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="26" t="s">
+      <c r="B15" s="26"/>
+      <c r="C15" s="17" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="24" t="s">
+      <c r="B16" s="26"/>
+      <c r="C16" s="26" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="17"/>
+      <c r="B17" s="21"/>
       <c r="C17" s="27" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="24" t="s">
+      <c r="B18" s="21"/>
+      <c r="C18" s="21" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="28" t="s">
+      <c r="B19" s="22"/>
+      <c r="C19" s="23" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="28" t="s">
+      <c r="B20" s="21"/>
+      <c r="C20" s="23" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="28" t="s">
+      <c r="B21" s="21"/>
+      <c r="C21" s="23" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" s="21"/>
+      <c r="C22" s="23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="17"/>
-      <c r="C22" s="24" t="s">
+      <c r="B23" s="21"/>
+      <c r="C23" s="21" t="s">
         <v>65</v>
       </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
08/02/2017 Update from Jimmy on issue 5
08/02/2017 Update from Jimmy on issue 5
</commit_message>
<xml_diff>
--- a/Gemalto-CloudGate-Issues_O.xlsx
+++ b/Gemalto-CloudGate-Issues_O.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="195" yWindow="660" windowWidth="26505" windowHeight="10590"/>
+    <workbookView xWindow="195" yWindow="660" windowWidth="20730" windowHeight="10590"/>
   </bookViews>
   <sheets>
     <sheet name="Issue Tracking" sheetId="1" r:id="rId1"/>
@@ -328,16 +328,6 @@
     <t>Having challenges activating on Verizon after GetWireless removed their Verizon plan.  Factory reseting not helping.  Brandon engaged.</t>
   </si>
   <si>
-    <t>•This is the same on both the current CG 3G (Gobi) and the CG LTE. There was no change compared to those devices.
-•We will try to get to a solution for the release following the 2.70.0. Some testing will be needed from GetWireless and Option.
-•Engineering build will be provided in January for testing and if OK, then a release will happen the same month.
-•01/06 Engineering build provided to GetWireless. GetWireless to test.
-•01/11 It will be great if we can get a result by the end of the week so that we can add it on the release candidate.
-•01/18 Jimmy is looking into this one.
-•01/25 There seems to be a problem with the modem that stays on SIM not ready and that is why is showing the problem after a radio modem reboot. We need to look ino the modem log and either fix it ourselves or get a fix from Gemalto.
-• 02/01 The BE team is still investigating the reason why the SIM command returns "SIM busy" after the modem reboot. It is not clear yet why this is happening. More investigation is needed.</t>
-  </si>
-  <si>
     <t>•Jimmy needs to have a teamviewer session to debug what is going on here.
 •11/28 Teamviewer ready for Jimmy.
 •11/29 Jimmy tested and saw a delay of 2 minutes when switching. He will investigate and see if there is any chance for improvement.
@@ -353,6 +343,14 @@
   </si>
   <si>
     <t>Available.</t>
+  </si>
+  <si>
+    <t>•01/06 Engineering build provided to GetWireless. GetWireless to test. (2.70.0)
+•01/11 It will be great if we can get a result by the end of the week so that we can add it on the release candidate.
+•01/18 Jimmy is looking into this one.
+•01/25 There seems to be a problem with the modem that stays on SIM not ready and that is why is showing the problem after a radio modem reboot. We need to look ino the modem log and either fix it ourselves or get a fix from Gemalto.
+• 02/01 The BE team is still investigating the reason why the SIM command returns "SIM busy" after the modem reboot. It is not clear yet why this is happening. More investigation is needed.
+• 02/08 The problem is related to a switch between SIM cards with different power levels (1.8V and 2.8V). This was found by the team in BE,  but at this point we need help from Gemalto.</t>
   </si>
 </sst>
 </file>
@@ -1031,9 +1029,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1201,7 +1199,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="390" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="330" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>5</v>
       </c>
@@ -1215,7 +1213,7 @@
         <v>31</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>66</v>
@@ -1244,7 +1242,7 @@
         <v>67</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="7" t="s">
@@ -1779,7 +1777,7 @@
       </c>
       <c r="B22" s="21"/>
       <c r="C22" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1793,7 +1791,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B24" s="21"/>
       <c r="C24" s="21"/>

</xml_diff>

<commit_message>
10/02/2017 Updated Customer Feedback tab after GW call.
10/02/2017 Updated Customer Feedback tab after GW call.
</commit_message>
<xml_diff>
--- a/Gemalto-CloudGate-Issues_O.xlsx
+++ b/Gemalto-CloudGate-Issues_O.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="195" yWindow="660" windowWidth="20730" windowHeight="10590"/>
+    <workbookView xWindow="195" yWindow="660" windowWidth="20730" windowHeight="10590" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Issue Tracking" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="100">
   <si>
     <t>Issue</t>
   </si>
@@ -240,9 +240,6 @@
     <t>Happy per comments above and device is returned.  Shipped to Pinnacle.</t>
   </si>
   <si>
-    <t>No update as of yet.</t>
-  </si>
-  <si>
     <t>Brandon testing</t>
   </si>
   <si>
@@ -314,18 +311,6 @@
   </si>
   <si>
     <t>Still no response from Sensaphone on request to send back unit.  Brandon pinging them daily and Truax following up.</t>
-  </si>
-  <si>
-    <t>Customer uses port forwarding to open up port 4000 on CG firewall; however when the TCP node in LuvitRED already opens the hole in the firewall on that port, serial device is not reachable.  He is retesting with Gobi based CloudGate per Franco's input. Offshore most of last week- just getting back to more testing.</t>
-  </si>
-  <si>
-    <t>Being used for a project design. Jonathan working to free it up and get it back.</t>
-  </si>
-  <si>
-    <t>Passed their tests.  Andrew working on tracking down if sent back yet.</t>
-  </si>
-  <si>
-    <t>Having challenges activating on Verizon after GetWireless removed their Verizon plan.  Factory reseting not helping.  Brandon engaged.</t>
   </si>
   <si>
     <t>•Jimmy needs to have a teamviewer session to debug what is going on here.
@@ -339,18 +324,45 @@
 •02/03 We sent a new log as requested by Gemalto.</t>
   </si>
   <si>
-    <t>New unit sent to them to evaluate; problem unit received back and being evaluated</t>
-  </si>
-  <si>
-    <t>Available.</t>
-  </si>
-  <si>
     <t>•01/06 Engineering build provided to GetWireless. GetWireless to test. (2.70.0)
 •01/11 It will be great if we can get a result by the end of the week so that we can add it on the release candidate.
 •01/18 Jimmy is looking into this one.
 •01/25 There seems to be a problem with the modem that stays on SIM not ready and that is why is showing the problem after a radio modem reboot. We need to look ino the modem log and either fix it ourselves or get a fix from Gemalto.
 • 02/01 The BE team is still investigating the reason why the SIM command returns "SIM busy" after the modem reboot. It is not clear yet why this is happening. More investigation is needed.
 • 02/08 The problem is related to a switch between SIM cards with different power levels (1.8V and 2.8V). This was found by the team in BE,  but at this point we need help from Gemalto.</t>
+  </si>
+  <si>
+    <t>Passed their tests.  Unit returned.</t>
+  </si>
+  <si>
+    <t>Option</t>
+  </si>
+  <si>
+    <t>Failed unit from Wanco sent back to Belgium today Fed Ex 778390395630.  Brandon tested and it was constantly rebooting every few seconds.</t>
+  </si>
+  <si>
+    <t>Customer uses port forwarding to open up port 4000 on CG firewall; however when the TCP node in LuvitRED already opens the hole in the firewall on that port, serial device is not reachable.  He is retesting with Gobi based CloudGate per Franco's input. Not getting responses to test status queries.</t>
+  </si>
+  <si>
+    <t>Being used for a project design. Jonathan checking if still providing value.</t>
+  </si>
+  <si>
+    <t>Working fine.  Being returned next week.</t>
+  </si>
+  <si>
+    <t>They are in the process of testing the new unit they just received.  All good so far.</t>
+  </si>
+  <si>
+    <t>2 for US Cellular</t>
+  </si>
+  <si>
+    <t>Global Phone - Nomad</t>
+  </si>
+  <si>
+    <t>New Ecology</t>
+  </si>
+  <si>
+    <t>Xylem</t>
   </si>
 </sst>
 </file>
@@ -386,7 +398,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -399,8 +411,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -473,11 +491,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -525,29 +554,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1029,8 +1061,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -1187,7 +1219,7 @@
         <v>61</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>23</v>
@@ -1213,10 +1245,10 @@
         <v>31</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>22</v>
@@ -1239,10 +1271,10 @@
         <v>40</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="7" t="s">
@@ -1326,7 +1358,7 @@
         <v>59</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>23</v>
@@ -1355,7 +1387,7 @@
         <v>53</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>23</v>
@@ -1384,7 +1416,7 @@
         <v>60</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>23</v>
@@ -1580,39 +1612,39 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="133.28515625" style="13" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="18"/>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="25" t="s">
+      <c r="A2" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="24" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" s="20">
         <v>42710</v>
@@ -1623,7 +1655,7 @@
     </row>
     <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" s="20">
         <v>42712</v>
@@ -1634,7 +1666,7 @@
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" s="20">
         <v>42717</v>
@@ -1645,7 +1677,7 @@
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" s="20">
         <v>42726</v>
@@ -1660,124 +1692,124 @@
       <c r="C7" s="19"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="25"/>
+      <c r="C12" s="26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="28" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
+      <c r="B13" s="27"/>
+      <c r="C13" s="25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="29"/>
-      <c r="C13" s="26" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
+      <c r="B14" s="25"/>
+      <c r="C14" s="25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
+      <c r="B15" s="25"/>
+      <c r="C15" s="28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="17" t="s">
+      <c r="B16" s="25"/>
+      <c r="C16" s="25" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="29"/>
+      <c r="C17" s="25" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" s="31"/>
+      <c r="C18" s="30" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
+      <c r="B19" s="21"/>
+      <c r="C19" s="18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="27" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="23" t="s">
+      <c r="B20" s="21"/>
+      <c r="C20" s="21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="B19" s="22"/>
-      <c r="C19" s="23" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="23" t="s">
+      <c r="B21" s="21"/>
+      <c r="C21" s="22" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="23" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="23" t="s">
-        <v>82</v>
-      </c>
       <c r="B22" s="21"/>
-      <c r="C22" s="23" t="s">
-        <v>93</v>
+      <c r="C22" s="22" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1786,15 +1818,41 @@
       </c>
       <c r="B23" s="21"/>
       <c r="C23" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="B24" s="21"/>
+      <c r="A24" s="32"/>
+      <c r="B24" s="17"/>
       <c r="C24" s="21"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
22/02/2017 Update after call with Thomas and GetWireless
22/02/2017 Update after call with Thomas and GetWireless
</commit_message>
<xml_diff>
--- a/Gemalto-CloudGate-Issues_O.xlsx
+++ b/Gemalto-CloudGate-Issues_O.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="195" yWindow="660" windowWidth="20730" windowHeight="10590" activeTab="2"/>
+    <workbookView xWindow="195" yWindow="660" windowWidth="20730" windowHeight="10590"/>
   </bookViews>
   <sheets>
     <sheet name="Issue Tracking" sheetId="1" r:id="rId1"/>
@@ -324,45 +324,46 @@
 •02/03 We sent a new log as requested by Gemalto.</t>
   </si>
   <si>
+    <t>Passed their tests.  Unit returned.</t>
+  </si>
+  <si>
+    <t>Option</t>
+  </si>
+  <si>
+    <t>Failed unit from Wanco sent back to Belgium today Fed Ex 778390395630.  Brandon tested and it was constantly rebooting every few seconds.</t>
+  </si>
+  <si>
+    <t>Customer uses port forwarding to open up port 4000 on CG firewall; however when the TCP node in LuvitRED already opens the hole in the firewall on that port, serial device is not reachable.  He is retesting with Gobi based CloudGate per Franco's input. Not getting responses to test status queries.</t>
+  </si>
+  <si>
+    <t>Being used for a project design. Jonathan checking if still providing value.</t>
+  </si>
+  <si>
+    <t>Working fine.  Being returned next week.</t>
+  </si>
+  <si>
+    <t>They are in the process of testing the new unit they just received.  All good so far.</t>
+  </si>
+  <si>
+    <t>2 for US Cellular</t>
+  </si>
+  <si>
+    <t>Global Phone - Nomad</t>
+  </si>
+  <si>
+    <t>New Ecology</t>
+  </si>
+  <si>
+    <t>Xylem</t>
+  </si>
+  <si>
     <t>•01/06 Engineering build provided to GetWireless. GetWireless to test. (2.70.0)
 •01/11 It will be great if we can get a result by the end of the week so that we can add it on the release candidate.
 •01/18 Jimmy is looking into this one.
 •01/25 There seems to be a problem with the modem that stays on SIM not ready and that is why is showing the problem after a radio modem reboot. We need to look ino the modem log and either fix it ourselves or get a fix from Gemalto.
 • 02/01 The BE team is still investigating the reason why the SIM command returns "SIM busy" after the modem reboot. It is not clear yet why this is happening. More investigation is needed.
-• 02/08 The problem is related to a switch between SIM cards with different power levels (1.8V and 2.8V). This was found by the team in BE,  but at this point we need help from Gemalto.</t>
-  </si>
-  <si>
-    <t>Passed their tests.  Unit returned.</t>
-  </si>
-  <si>
-    <t>Option</t>
-  </si>
-  <si>
-    <t>Failed unit from Wanco sent back to Belgium today Fed Ex 778390395630.  Brandon tested and it was constantly rebooting every few seconds.</t>
-  </si>
-  <si>
-    <t>Customer uses port forwarding to open up port 4000 on CG firewall; however when the TCP node in LuvitRED already opens the hole in the firewall on that port, serial device is not reachable.  He is retesting with Gobi based CloudGate per Franco's input. Not getting responses to test status queries.</t>
-  </si>
-  <si>
-    <t>Being used for a project design. Jonathan checking if still providing value.</t>
-  </si>
-  <si>
-    <t>Working fine.  Being returned next week.</t>
-  </si>
-  <si>
-    <t>They are in the process of testing the new unit they just received.  All good so far.</t>
-  </si>
-  <si>
-    <t>2 for US Cellular</t>
-  </si>
-  <si>
-    <t>Global Phone - Nomad</t>
-  </si>
-  <si>
-    <t>New Ecology</t>
-  </si>
-  <si>
-    <t>Xylem</t>
+• 02/08 The problem is related to a switch between SIM cards with different power levels (1.8V and 2.8V). This was found by the team in BE,  but at this point we need help from Gemalto.
+• 02/22 We are planning to sent a SIM card to Gemalto if they are not able to find one at their end that works with 2.8V.</t>
   </si>
 </sst>
 </file>
@@ -1061,9 +1062,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1231,7 +1232,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="330" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="375" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>5</v>
       </c>
@@ -1245,7 +1246,7 @@
         <v>31</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>65</v>
@@ -1614,8 +1615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1764,16 +1765,16 @@
       </c>
       <c r="B17" s="29"/>
       <c r="C17" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B18" s="31"/>
       <c r="C18" s="30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -1782,7 +1783,7 @@
       </c>
       <c r="B19" s="21"/>
       <c r="C19" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1791,7 +1792,7 @@
       </c>
       <c r="B20" s="21"/>
       <c r="C20" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1800,7 +1801,7 @@
       </c>
       <c r="B21" s="21"/>
       <c r="C21" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1809,7 +1810,7 @@
       </c>
       <c r="B22" s="21"/>
       <c r="C22" s="22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1828,28 +1829,28 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B26" s="21"/>
       <c r="C26" s="21"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B27" s="21"/>
       <c r="C27" s="21"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B28" s="21"/>
       <c r="C28" s="21"/>

</xml_diff>

<commit_message>
01/03/2017 Updates from Thomas.
01/03/2017 Updates from Thomas.
</commit_message>
<xml_diff>
--- a/Gemalto-CloudGate-Issues_O.xlsx
+++ b/Gemalto-CloudGate-Issues_O.xlsx
@@ -313,57 +313,57 @@
     <t>Still no response from Sensaphone on request to send back unit.  Brandon pinging them daily and Truax following up.</t>
   </si>
   <si>
-    <t>•Jimmy needs to have a teamviewer session to debug what is going on here.
-•11/28 Teamviewer ready for Jimmy.
+    <t>Passed their tests.  Unit returned.</t>
+  </si>
+  <si>
+    <t>Option</t>
+  </si>
+  <si>
+    <t>Failed unit from Wanco sent back to Belgium today Fed Ex 778390395630.  Brandon tested and it was constantly rebooting every few seconds.</t>
+  </si>
+  <si>
+    <t>Customer uses port forwarding to open up port 4000 on CG firewall; however when the TCP node in LuvitRED already opens the hole in the firewall on that port, serial device is not reachable.  He is retesting with Gobi based CloudGate per Franco's input. Not getting responses to test status queries.</t>
+  </si>
+  <si>
+    <t>Being used for a project design. Jonathan checking if still providing value.</t>
+  </si>
+  <si>
+    <t>Working fine.  Being returned next week.</t>
+  </si>
+  <si>
+    <t>They are in the process of testing the new unit they just received.  All good so far.</t>
+  </si>
+  <si>
+    <t>2 for US Cellular</t>
+  </si>
+  <si>
+    <t>Global Phone - Nomad</t>
+  </si>
+  <si>
+    <t>New Ecology</t>
+  </si>
+  <si>
+    <t>Xylem</t>
+  </si>
+  <si>
+    <t>•01/06 Eng. build for GW to test. (2.70.0)
+•01/11 It will be great if we can get a result by the end of the week so that we can add it on the release candidate.
+•01/18 Jimmy is looking into this one.
+•01/25 There seems to be a problem with the modem that stays on SIM not ready and that is why is showing the problem after a radio modem reboot. We need to look ino the modem log and either fix it ourselves or get a fix from Gemalto.
+• 02/01 The BE team investigating the reason for SIM command returning "SIM busy" after the modem reboot. More investigation is needed.
+• 02/08 The problem is related to a switch between SIM cards with different power levels (1.8V and 2.8V). This was found by the team in BE,  but at this point we need help from Gemalto.
+• 02/22 We are planning to sent a SIM card to Gemalto if they are not able to find one at their end that works with 2.8V.
+• 03/01 SIM is being send to Gemalto Poland for investigation. Gemalto stated they don't have locally a SIM that works with 2.8V, so we need to send ours.</t>
+  </si>
+  <si>
+    <t>•11/28 Teamviewer ready for Jimmy.
 •11/29 Jimmy tested and saw a delay of 2 minutes when switching. He will investigate and see if there is any chance for improvement.
-•There is a problem with this setup being offline every day. Jimmy is loosing time as he cannot test without an active TV.
 •01/04 Jimmy is going to try to see the same issue in Belgium and if he does the TV setup will no longer be needed.
 •01/11 The issue does not seem to be related to the firmware switch, but to something specific on the SIM. We are asking Gemalto to check this on the module.
 •01/18 We are waiting feedback from Gemalto on this one. They are looking into it, but might take time.
 •02/01 Gemalto is asking for a new, more complicated log to get some more data about the issue, but this log is proving to be a complicated one. The BE team is working to get the log for them.
-•02/03 We sent a new log as requested by Gemalto.</t>
-  </si>
-  <si>
-    <t>Passed their tests.  Unit returned.</t>
-  </si>
-  <si>
-    <t>Option</t>
-  </si>
-  <si>
-    <t>Failed unit from Wanco sent back to Belgium today Fed Ex 778390395630.  Brandon tested and it was constantly rebooting every few seconds.</t>
-  </si>
-  <si>
-    <t>Customer uses port forwarding to open up port 4000 on CG firewall; however when the TCP node in LuvitRED already opens the hole in the firewall on that port, serial device is not reachable.  He is retesting with Gobi based CloudGate per Franco's input. Not getting responses to test status queries.</t>
-  </si>
-  <si>
-    <t>Being used for a project design. Jonathan checking if still providing value.</t>
-  </si>
-  <si>
-    <t>Working fine.  Being returned next week.</t>
-  </si>
-  <si>
-    <t>They are in the process of testing the new unit they just received.  All good so far.</t>
-  </si>
-  <si>
-    <t>2 for US Cellular</t>
-  </si>
-  <si>
-    <t>Global Phone - Nomad</t>
-  </si>
-  <si>
-    <t>New Ecology</t>
-  </si>
-  <si>
-    <t>Xylem</t>
-  </si>
-  <si>
-    <t>•01/06 Engineering build provided to GetWireless. GetWireless to test. (2.70.0)
-•01/11 It will be great if we can get a result by the end of the week so that we can add it on the release candidate.
-•01/18 Jimmy is looking into this one.
-•01/25 There seems to be a problem with the modem that stays on SIM not ready and that is why is showing the problem after a radio modem reboot. We need to look ino the modem log and either fix it ourselves or get a fix from Gemalto.
-• 02/01 The BE team is still investigating the reason why the SIM command returns "SIM busy" after the modem reboot. It is not clear yet why this is happening. More investigation is needed.
-• 02/08 The problem is related to a switch between SIM cards with different power levels (1.8V and 2.8V). This was found by the team in BE,  but at this point we need help from Gemalto.
-• 02/22 We are planning to sent a SIM card to Gemalto if they are not able to find one at their end that works with 2.8V.</t>
+•02/03 We sent a new log as requested by Gemalto.
+• 03/01 We have a fix for this issue that will be included on the next release (2.75.0) that will be available in 3.5 weeks.</t>
   </si>
 </sst>
 </file>
@@ -1064,7 +1064,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1232,7 +1232,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="375" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="405" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>5</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>31</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>65</v>
@@ -1261,7 +1261,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="405" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="375" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>6</v>
       </c>
@@ -1275,7 +1275,7 @@
         <v>66</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="7" t="s">
@@ -1765,16 +1765,16 @@
       </c>
       <c r="B17" s="29"/>
       <c r="C17" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B18" s="31"/>
       <c r="C18" s="30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -1783,7 +1783,7 @@
       </c>
       <c r="B19" s="21"/>
       <c r="C19" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1792,7 +1792,7 @@
       </c>
       <c r="B20" s="21"/>
       <c r="C20" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1801,7 +1801,7 @@
       </c>
       <c r="B21" s="21"/>
       <c r="C21" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1810,7 +1810,7 @@
       </c>
       <c r="B22" s="21"/>
       <c r="C22" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1829,28 +1829,28 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B26" s="21"/>
       <c r="C26" s="21"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B27" s="21"/>
       <c r="C27" s="21"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B28" s="21"/>
       <c r="C28" s="21"/>

</xml_diff>

<commit_message>
01/03/2017 Change on issue #6 new firmware.
01/03/2017 Change on issue #6 new firmware.
</commit_message>
<xml_diff>
--- a/Gemalto-CloudGate-Issues_O.xlsx
+++ b/Gemalto-CloudGate-Issues_O.xlsx
@@ -1062,9 +1062,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1279,7 +1279,7 @@
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
08/03/207 Updates from Thomas.
08/03/207 Updates from Thomas.
</commit_message>
<xml_diff>
--- a/Gemalto-CloudGate-Issues_O.xlsx
+++ b/Gemalto-CloudGate-Issues_O.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Customer Feedback" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Issue Tracking'!$G$1:$G$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Issue Tracking'!$G$1:$G$15</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="103">
   <si>
     <t>Issue</t>
   </si>
@@ -344,16 +344,6 @@
   </si>
   <si>
     <t>Xylem</t>
-  </si>
-  <si>
-    <t>•01/06 Eng. build for GW to test. (2.70.0)
-•01/11 It will be great if we can get a result by the end of the week so that we can add it on the release candidate.
-•01/18 Jimmy is looking into this one.
-•01/25 There seems to be a problem with the modem that stays on SIM not ready and that is why is showing the problem after a radio modem reboot. We need to look ino the modem log and either fix it ourselves or get a fix from Gemalto.
-• 02/01 The BE team investigating the reason for SIM command returning "SIM busy" after the modem reboot. More investigation is needed.
-• 02/08 The problem is related to a switch between SIM cards with different power levels (1.8V and 2.8V). This was found by the team in BE,  but at this point we need help from Gemalto.
-• 02/22 We are planning to sent a SIM card to Gemalto if they are not able to find one at their end that works with 2.8V.
-• 03/01 SIM is being send to Gemalto Poland for investigation. Gemalto stated they don't have locally a SIM that works with 2.8V, so we need to send ours.</t>
   </si>
   <si>
     <t>•11/28 Teamviewer ready for Jimmy.
@@ -364,6 +354,24 @@
 •02/01 Gemalto is asking for a new, more complicated log to get some more data about the issue, but this log is proving to be a complicated one. The BE team is working to get the log for them.
 •02/03 We sent a new log as requested by Gemalto.
 • 03/01 We have a fix for this issue that will be included on the next release (2.75.0) that will be available in 3.5 weeks.</t>
+  </si>
+  <si>
+    <t>•01/06 Eng. build for GW to test. (2.70.0)
+•01/25 There seems to be a problem with the modem that stays on SIM not ready and that is why is showing the problem after a radio modem reboot. We need to look ino the modem log and either fix it ourselves or get a fix from Gemalto.
+• 02/01 The BE team investigating the reason for SIM command returning "SIM busy" after the modem reboot. More investigation is needed.
+• 02/08 The problem is related to a switch between SIM cards with different power levels (1.8V and 2.8V). This was found by the team in BE,  but at this point we need help from Gemalto.
+• 02/22 We are planning to sent a SIM card to Gemalto if they are not able to find one at their end that works with 2.8V.
+• 03/01 SIM is being send to Gemalto Poland for investigation. Gemalto stated they don't have locally a SIM that works with 2.8V, so we need to send ours.
+• 03/08 We might have a solution from Gemalto. We still need to test it, but if everything is OK we will include a fix on the next release (2.75.0)</t>
+  </si>
+  <si>
+    <t>• 03/08 We are working on a fix that should make the next firmware release (2.75.0).</t>
+  </si>
+  <si>
+    <t>Downgrade to very old firmware version is possible on Gemalto, but this causes the device to not respond as the power control is not in place</t>
+  </si>
+  <si>
+    <t>• A new feature will be added to not allow downgrade to firmware older than 2.70.0</t>
   </si>
 </sst>
 </file>
@@ -507,13 +515,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -581,6 +586,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1060,242 +1071,242 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="80.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="42.85546875" style="6" customWidth="1"/>
-    <col min="6" max="6" width="32.28515625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="80.28515625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="42.85546875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="32.28515625" style="5" customWidth="1"/>
     <col min="7" max="7" width="24.7109375" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
     <col min="9" max="9" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-    </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="2" t="s">
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:9" s="33" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="32" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11">
+      <c r="A3" s="10">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="120" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
+      <c r="A4" s="10">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
+      <c r="A5" s="10">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
+      <c r="A6" s="10">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="405" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
+      <c r="A7" s="10">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>98</v>
+      <c r="E7" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="8" t="s">
+      <c r="G7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="375" x14ac:dyDescent="0.25">
-      <c r="A8" s="11">
+      <c r="A8" s="10">
         <v>6</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>66</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11">
+      <c r="A9" s="10">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1305,24 +1316,24 @@
         <v>56</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I9" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
+      <c r="A10" s="10">
         <v>8</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1332,24 +1343,24 @@
         <v>57</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I10" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
+      <c r="A11" s="10">
         <v>9</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1358,27 +1369,27 @@
       <c r="E11" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="210" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11">
+      <c r="A12" s="10">
         <v>10</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -1387,27 +1398,27 @@
       <c r="E12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I12" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="150" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11">
+      <c r="A13" s="10">
         <v>11</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1419,37 +1430,64 @@
       <c r="F13" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="I13" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="4" t="s">
+    <row r="14" spans="1:9" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="F14" s="14"/>
+      <c r="G14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8" t="s">
+      <c r="C15" s="3"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="G1:G14">
+  <autoFilter ref="G1:G15">
     <filterColumn colId="0">
       <filters blank="1">
+        <filter val="New firmware"/>
         <filter val="Status"/>
-        <filter val="Under Investigation (OP)"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -1464,7 +1502,7 @@
       <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H10:H13">
+  <conditionalFormatting sqref="H10:H14">
     <cfRule type="cellIs" dxfId="12" priority="25" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
@@ -1475,7 +1513,7 @@
       <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H14">
+  <conditionalFormatting sqref="H15">
     <cfRule type="cellIs" dxfId="9" priority="22" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
@@ -1486,7 +1524,7 @@
       <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G14">
+  <conditionalFormatting sqref="G3:G15">
     <cfRule type="expression" dxfId="6" priority="19">
       <formula>ISNUMBER(SEARCH("Under",G3))</formula>
     </cfRule>
@@ -1497,12 +1535,12 @@
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G14">
+  <conditionalFormatting sqref="G3:G15">
     <cfRule type="cellIs" dxfId="3" priority="18" operator="equal">
       <formula>"New firmware"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I14">
+  <conditionalFormatting sqref="I3:I15">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
@@ -1522,19 +1560,19 @@
           <x14:formula1>
             <xm:f>Legend!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>H3:H14</xm:sqref>
+          <xm:sqref>H3:H15</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Legend!$C$2:$C$8</xm:f>
           </x14:formula1>
-          <xm:sqref>G3:G14</xm:sqref>
+          <xm:sqref>G3:G15</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Legend!$D$2:$D$3</xm:f>
           </x14:formula1>
-          <xm:sqref>I3:I14</xm:sqref>
+          <xm:sqref>I3:I15</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1621,239 +1659,239 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="133.28515625" style="13" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="13"/>
+    <col min="1" max="1" width="21.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="133.28515625" style="12" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="17"/>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
+      <c r="A1" s="16"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="23" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" s="19">
         <v>42710</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="18" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="19">
         <v>42712</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="19">
         <v>42717</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="18" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="B6" s="20">
+      <c r="B6" s="19">
         <v>42726</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="18" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="26" t="s">
+      <c r="B12" s="24"/>
+      <c r="C12" s="25" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="27"/>
-      <c r="C13" s="25" t="s">
+      <c r="B13" s="26"/>
+      <c r="C13" s="24" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25" t="s">
+      <c r="B14" s="24"/>
+      <c r="C14" s="24" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="28" t="s">
+      <c r="B15" s="24"/>
+      <c r="C15" s="27" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25" t="s">
+      <c r="B16" s="24"/>
+      <c r="C16" s="24" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="25" t="s">
+      <c r="B17" s="28"/>
+      <c r="C17" s="24" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="B18" s="31"/>
-      <c r="C18" s="30" t="s">
+      <c r="B18" s="30"/>
+      <c r="C18" s="29" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="18" t="s">
+      <c r="B19" s="20"/>
+      <c r="C19" s="17" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21" t="s">
+      <c r="B20" s="20"/>
+      <c r="C20" s="20" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="22" t="s">
+      <c r="B21" s="20"/>
+      <c r="C21" s="21" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="B22" s="21"/>
-      <c r="C22" s="22" t="s">
+      <c r="B22" s="20"/>
+      <c r="C22" s="21" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21" t="s">
+      <c r="B23" s="20"/>
+      <c r="C23" s="20" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="21"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="20"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
17/03/2017 Update after GW call.
17/03/2017 Update after GW call.
</commit_message>
<xml_diff>
--- a/Gemalto-CloudGate-Issues_O.xlsx
+++ b/Gemalto-CloudGate-Issues_O.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="105">
   <si>
     <t>Issue</t>
   </si>
@@ -240,9 +240,6 @@
     <t>Happy per comments above and device is returned.  Shipped to Pinnacle.</t>
   </si>
   <si>
-    <t>Brandon testing</t>
-  </si>
-  <si>
     <t>•01/13 Brandon saw a problem with the modem not reading the SIM correctly after switching it and rebooting the modem.</t>
   </si>
   <si>
@@ -322,28 +319,10 @@
     <t>Failed unit from Wanco sent back to Belgium today Fed Ex 778390395630.  Brandon tested and it was constantly rebooting every few seconds.</t>
   </si>
   <si>
-    <t>Customer uses port forwarding to open up port 4000 on CG firewall; however when the TCP node in LuvitRED already opens the hole in the firewall on that port, serial device is not reachable.  He is retesting with Gobi based CloudGate per Franco's input. Not getting responses to test status queries.</t>
-  </si>
-  <si>
     <t>Being used for a project design. Jonathan checking if still providing value.</t>
   </si>
   <si>
-    <t>Working fine.  Being returned next week.</t>
-  </si>
-  <si>
     <t>They are in the process of testing the new unit they just received.  All good so far.</t>
-  </si>
-  <si>
-    <t>2 for US Cellular</t>
-  </si>
-  <si>
-    <t>Global Phone - Nomad</t>
-  </si>
-  <si>
-    <t>New Ecology</t>
-  </si>
-  <si>
-    <t>Xylem</t>
   </si>
   <si>
     <t>•11/28 Teamviewer ready for Jimmy.
@@ -372,6 +351,33 @@
   </si>
   <si>
     <t>• A new feature will be added to not allow downgrade to firmware older than 2.70.0</t>
+  </si>
+  <si>
+    <t>Returned unit.  Will not be a reseller without C1D2.</t>
+  </si>
+  <si>
+    <t>Jonathan</t>
+  </si>
+  <si>
+    <t>Working fine.  Returned.</t>
+  </si>
+  <si>
+    <t>Jim Wagner</t>
+  </si>
+  <si>
+    <t>Freight Farms</t>
+  </si>
+  <si>
+    <t>Ron Vener</t>
+  </si>
+  <si>
+    <t>Testing in Process.</t>
+  </si>
+  <si>
+    <t>Baseline</t>
+  </si>
+  <si>
+    <t>Steve Koontz</t>
   </si>
 </sst>
 </file>
@@ -515,7 +521,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -561,9 +567,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -586,11 +597,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1100,30 +1108,30 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:9" s="33" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="18" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="32" t="s">
+      <c r="H2" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="I2" s="17" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1231,7 +1239,7 @@
         <v>61</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>23</v>
@@ -1257,10 +1265,10 @@
         <v>31</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>24</v>
@@ -1283,10 +1291,10 @@
         <v>40</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="6" t="s">
@@ -1370,7 +1378,7 @@
         <v>59</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>23</v>
@@ -1399,7 +1407,7 @@
         <v>53</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>23</v>
@@ -1428,7 +1436,7 @@
         <v>60</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>23</v>
@@ -1445,16 +1453,16 @@
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F14" s="14"/>
       <c r="G14" s="6" t="s">
@@ -1651,247 +1659,256 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="133.28515625" style="12" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="16"/>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
+      <c r="A1" s="20"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="B3" s="22">
+        <v>42710</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="19">
-        <v>42710</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="B4" s="22">
+        <v>42712</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="19">
-        <v>42712</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="B5" s="22">
+        <v>42717</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="19">
-        <v>42717</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="B6" s="22">
+        <v>42726</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="B6" s="19">
-        <v>42726</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="27"/>
+      <c r="C12" s="28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="25" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
+      <c r="B13" s="29"/>
+      <c r="C13" s="27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="24" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
+      <c r="B14" s="27"/>
+      <c r="C14" s="27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
+      <c r="B15" s="27"/>
+      <c r="C15" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="27" t="s">
+      <c r="B16" s="27"/>
+      <c r="C16" s="27" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="31"/>
+      <c r="C17" s="27" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="33"/>
+      <c r="C18" s="32" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
+      <c r="B19" s="27"/>
+      <c r="C19" s="35" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="B17" s="28"/>
-      <c r="C17" s="24" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="B18" s="30"/>
-      <c r="C18" s="29" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="17" t="s">
+      <c r="B21" s="27"/>
+      <c r="C21" s="27" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" s="24" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="21" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="B22" s="20"/>
-      <c r="C22" s="21" t="s">
-        <v>93</v>
-      </c>
-    </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20" t="s">
-        <v>64</v>
+      <c r="A23" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" s="23" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="31"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="20"/>
+      <c r="A24" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
+      <c r="A28" s="19"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="19"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
31/03/2017 Update after Getwireless call.
31/03/2017 Update after Getwireless call.
</commit_message>
<xml_diff>
--- a/Gemalto-CloudGate-Issues_O.xlsx
+++ b/Gemalto-CloudGate-Issues_O.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="195" yWindow="660" windowWidth="20730" windowHeight="10590"/>
+    <workbookView xWindow="195" yWindow="660" windowWidth="20730" windowHeight="10590" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Issue Tracking" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="108">
   <si>
     <t>Issue</t>
   </si>
@@ -320,9 +320,6 @@
   </si>
   <si>
     <t>Being used for a project design. Jonathan checking if still providing value.</t>
-  </si>
-  <si>
-    <t>They are in the process of testing the new unit they just received.  All good so far.</t>
   </si>
   <si>
     <t>•11/28 Teamviewer ready for Jimmy.
@@ -378,6 +375,18 @@
   </si>
   <si>
     <t>Steve Koontz</t>
+  </si>
+  <si>
+    <t>Jeremy Glen</t>
+  </si>
+  <si>
+    <t>Testing complete and no issues.  Unit is now being returned.</t>
+  </si>
+  <si>
+    <t>TCS Basys Controls</t>
+  </si>
+  <si>
+    <t>Unit enroute for testing</t>
   </si>
 </sst>
 </file>
@@ -1081,7 +1090,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
@@ -1265,7 +1274,7 @@
         <v>31</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>64</v>
@@ -1294,7 +1303,7 @@
         <v>65</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="6" t="s">
@@ -1453,16 +1462,16 @@
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F14" s="14"/>
       <c r="G14" s="6" t="s">
@@ -1661,8 +1670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1829,66 +1838,74 @@
       </c>
       <c r="B19" s="27"/>
       <c r="C19" s="35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="B20" s="23" t="s">
+      <c r="A20" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" s="27" t="s">
         <v>97</v>
-      </c>
-      <c r="C20" s="23" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="B21" s="27"/>
+        <v>80</v>
+      </c>
+      <c r="B21" s="27" t="s">
+        <v>98</v>
+      </c>
       <c r="C21" s="27" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="24" t="s">
-        <v>80</v>
+      <c r="A22" s="23" t="s">
+        <v>77</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="C22" s="24" t="s">
-        <v>90</v>
+        <v>96</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="C23" s="23" t="s">
         <v>101</v>
-      </c>
-      <c r="C23" s="23" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="B24" s="23" t="s">
-        <v>104</v>
-      </c>
       <c r="C24" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="19"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
+      <c r="A25" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>

</xml_diff>